<commit_message>
docs: modification de la documentation: documentation du jour 2
</commit_message>
<xml_diff>
--- a/docs/plannification_TPI.xlsx
+++ b/docs/plannification_TPI.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoann\Documents\Monogame\MiFiSy\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoann\Documents\Monogame\MiFiSy\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -150,7 +150,7 @@
     <numFmt numFmtId="164" formatCode="[hh]:mm"/>
     <numFmt numFmtId="165" formatCode="dd/mm"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,8 +199,15 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,8 +226,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -403,11 +415,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -518,6 +546,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -527,14 +558,18 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="18" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Insatisfaisant" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="356">
+  <dxfs count="284">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -632,6 +667,64 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -650,8 +743,24 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFC6D9F0"/>
           <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -688,14 +797,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -744,22 +845,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -792,6 +877,14 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -840,22 +933,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -888,6 +965,30 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -936,22 +1037,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -984,6 +1069,14 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -1008,14 +1101,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -1049,25 +1134,21 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1106,6 +1187,108 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFB8CCE4"/>
           <bgColor rgb="FFB8CCE4"/>
         </patternFill>
@@ -1130,6 +1313,30 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFC6D9F0"/>
           <bgColor rgb="FFC6D9F0"/>
         </patternFill>
@@ -1240,6 +1447,64 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -1258,8 +1523,24 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFC6D9F0"/>
           <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1296,14 +1577,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -1336,6 +1609,46 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFB8CCE4"/>
@@ -1346,16 +1659,248 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFB8CCE4"/>
           <bgColor rgb="FFB8CCE4"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFB8CCE4"/>
           <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1378,18 +1923,20 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFB8CCE4"/>
           <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1412,6 +1959,22 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFB8CCE4"/>
           <bgColor rgb="FFB8CCE4"/>
         </patternFill>
@@ -1420,6 +1983,76 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFC6D9F0"/>
           <bgColor rgb="FFC6D9F0"/>
         </patternFill>
@@ -1428,8 +2061,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1460,1187 +2093,25 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFC6D9F0"/>
           <bgColor rgb="FFC6D9F0"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFB8CCE4"/>
           <bgColor rgb="FFB8CCE4"/>
         </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
       </fill>
     </dxf>
     <dxf>
@@ -3621,7 +3092,7 @@
   <dimension ref="A1:AF1004"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3848,11 +3319,11 @@
       </c>
     </row>
     <row r="6" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
       <c r="D6" s="22"/>
       <c r="E6" s="18"/>
       <c r="F6" s="22"/>
@@ -4140,14 +3611,14 @@
       <c r="AF13" s="11"/>
     </row>
     <row r="14" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
       <c r="G14" s="18"/>
       <c r="H14" s="22"/>
       <c r="I14" s="18"/>
@@ -4392,17 +3863,17 @@
       </c>
     </row>
     <row r="22" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="45"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="45"/>
-      <c r="G22" s="45"/>
-      <c r="H22" s="45"/>
-      <c r="I22" s="45"/>
+      <c r="B22" s="46"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="46"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="46"/>
       <c r="J22" s="22"/>
       <c r="K22" s="22"/>
       <c r="L22" s="18"/>
@@ -4757,21 +4228,21 @@
       <c r="AF30" s="11"/>
     </row>
     <row r="31" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="44" t="s">
+      <c r="A31" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="45"/>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="45"/>
-      <c r="K31" s="45"/>
-      <c r="L31" s="45"/>
-      <c r="M31" s="46"/>
+      <c r="B31" s="46"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="46"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="46"/>
+      <c r="I31" s="46"/>
+      <c r="J31" s="46"/>
+      <c r="K31" s="46"/>
+      <c r="L31" s="46"/>
+      <c r="M31" s="47"/>
     </row>
     <row r="32" spans="1:32" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="33" t="s">
@@ -4915,7 +4386,7 @@
       </c>
     </row>
     <row r="35" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F35" s="47" t="s">
+      <c r="F35" s="44" t="s">
         <v>28</v>
       </c>
     </row>
@@ -5916,462 +5387,462 @@
     <mergeCell ref="A14:F14"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:J3 C26:C27 I26:I27 L2:M3 E26:E27 G26:G27 L26:L27 L8:L13 I8:I13 G8:G13 E8:E13 C8:C13 L19 I19 G19 E19 C19 C4:C5 E4:E6 G4:G6 I4:I6 L4:L6 C23 C16:C17 E23 E16:E17 G23 G16:G17 I23 I16:I17 L23 L16:L17 I30 I32 L30 L32 G30 G32 E30 E32 C30 C32">
-    <cfRule type="cellIs" dxfId="355" priority="194" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="283" priority="194" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:M13 C25:M27 C19:M19 C2:M5 C23:M23 C16:M17 D6:M6 L32:M32 C30:M30 C32:J32">
-    <cfRule type="cellIs" dxfId="354" priority="195" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="282" priority="195" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L25 I25 G25 E25 C25">
-    <cfRule type="cellIs" dxfId="353" priority="196" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="281" priority="196" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:J25 L25:M25">
-    <cfRule type="cellIs" dxfId="352" priority="197" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="280" priority="197" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30 F30 H30 J30 M30">
-    <cfRule type="cellIs" dxfId="351" priority="198" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="279" priority="198" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:M13 C25:M27 C19:M19 C2:M5 C23:M23 C16:M17 D6:M6 L32:M32 C30:M30 C32:J32">
-    <cfRule type="cellIs" dxfId="350" priority="201" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="278" priority="201" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:M13 C25:M27 C19:M19 C2:M5 C23:M23 C16:M17 D6:M6 L32:M32 C30:M30 C32:J32">
-    <cfRule type="cellIs" dxfId="349" priority="202" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="277" priority="202" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K3">
-    <cfRule type="cellIs" dxfId="348" priority="186" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="276" priority="186" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K3 K9:K13 K26:K27 K17 K30">
-    <cfRule type="cellIs" dxfId="347" priority="187" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="275" priority="187" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K25">
-    <cfRule type="cellIs" dxfId="346" priority="188" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="274" priority="188" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="cellIs" dxfId="345" priority="189" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="273" priority="189" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3 N25:N27 N5 N19 N21 N8:N13 N15:N17 N23 N30 N32">
-    <cfRule type="cellIs" dxfId="344" priority="184" operator="equal">
+    <cfRule type="cellIs" dxfId="272" priority="184" operator="equal">
       <formula>$B3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="cellIs" dxfId="343" priority="181" operator="equal">
+    <cfRule type="cellIs" dxfId="271" priority="181" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33:M33">
-    <cfRule type="cellIs" dxfId="342" priority="180" operator="equal">
+    <cfRule type="cellIs" dxfId="270" priority="180" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32">
-    <cfRule type="cellIs" dxfId="341" priority="177" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="269" priority="177" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F32">
-    <cfRule type="cellIs" dxfId="340" priority="176" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="268" priority="176" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="cellIs" dxfId="339" priority="175" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="267" priority="175" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J32">
-    <cfRule type="cellIs" dxfId="338" priority="174" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="266" priority="174" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="337" priority="169" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="265" priority="169" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="336" priority="170" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="264" priority="170" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="335" priority="171" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="263" priority="171" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="334" priority="172" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="262" priority="172" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="333" priority="173" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="261" priority="173" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M32">
-    <cfRule type="cellIs" dxfId="332" priority="168" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="260" priority="168" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2">
-    <cfRule type="cellIs" dxfId="331" priority="167" operator="equal">
+    <cfRule type="cellIs" dxfId="259" priority="167" operator="equal">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4">
-    <cfRule type="cellIs" dxfId="330" priority="166" operator="equal">
+    <cfRule type="cellIs" dxfId="258" priority="166" operator="equal">
       <formula>$B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7 E7 G7 I7 L7">
-    <cfRule type="cellIs" dxfId="329" priority="162" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="257" priority="162" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:J7 L7:M7">
-    <cfRule type="cellIs" dxfId="328" priority="163" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="256" priority="163" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:J7 L7:M7">
-    <cfRule type="cellIs" dxfId="327" priority="164" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="255" priority="164" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:J7 L7:M7">
-    <cfRule type="cellIs" dxfId="326" priority="165" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="254" priority="165" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="325" priority="159" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="253" priority="159" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="324" priority="160" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="252" priority="160" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="323" priority="161" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="251" priority="161" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="322" priority="152" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="250" priority="152" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18 E18 G18 I18 L18">
-    <cfRule type="cellIs" dxfId="321" priority="155" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="249" priority="155" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:J18 L18:M18">
-    <cfRule type="cellIs" dxfId="320" priority="156" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="248" priority="156" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:J18 L18:M18">
-    <cfRule type="cellIs" dxfId="319" priority="157" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="247" priority="157" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:J18 L18:M18">
-    <cfRule type="cellIs" dxfId="318" priority="158" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="246" priority="158" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="317" priority="153" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="245" priority="153" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="316" priority="154" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="244" priority="154" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L21 I21 G21 E21 C21">
-    <cfRule type="cellIs" dxfId="315" priority="143" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="243" priority="143" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:M21">
-    <cfRule type="cellIs" dxfId="314" priority="144" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="242" priority="144" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:M21">
-    <cfRule type="cellIs" dxfId="313" priority="145" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="241" priority="145" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:M21">
-    <cfRule type="cellIs" dxfId="312" priority="146" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="240" priority="146" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21">
-    <cfRule type="cellIs" dxfId="311" priority="142" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="239" priority="142" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="cellIs" dxfId="310" priority="134" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="238" priority="134" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28">
-    <cfRule type="cellIs" dxfId="309" priority="121" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="237" priority="121" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20 E20 G20 I20 L20">
-    <cfRule type="cellIs" dxfId="308" priority="137" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="236" priority="137" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:J20 L20:M20">
-    <cfRule type="cellIs" dxfId="307" priority="138" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="235" priority="138" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:J20 L20:M20">
-    <cfRule type="cellIs" dxfId="306" priority="139" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="234" priority="139" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:J20 L20:M20">
-    <cfRule type="cellIs" dxfId="305" priority="140" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="233" priority="140" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="cellIs" dxfId="304" priority="135" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="232" priority="135" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="cellIs" dxfId="303" priority="136" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="231" priority="136" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L15 I15 G15 E15 C15">
-    <cfRule type="cellIs" dxfId="302" priority="130" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="230" priority="130" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:M15">
-    <cfRule type="cellIs" dxfId="301" priority="131" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="229" priority="131" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:M15">
-    <cfRule type="cellIs" dxfId="300" priority="132" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="228" priority="132" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:M15">
-    <cfRule type="cellIs" dxfId="299" priority="133" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="227" priority="133" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="cellIs" dxfId="298" priority="129" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="226" priority="129" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28 E28 G28 I28 L28">
-    <cfRule type="cellIs" dxfId="297" priority="124" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="225" priority="124" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:J28 L28:M28">
-    <cfRule type="cellIs" dxfId="296" priority="125" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="224" priority="125" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:J28 L28:M28">
-    <cfRule type="cellIs" dxfId="295" priority="126" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="223" priority="126" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:J28 L28:M28">
-    <cfRule type="cellIs" dxfId="294" priority="127" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="222" priority="127" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28">
-    <cfRule type="cellIs" dxfId="293" priority="122" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="221" priority="122" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28">
-    <cfRule type="cellIs" dxfId="292" priority="123" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="220" priority="123" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24 E24 G24 I24 L24">
-    <cfRule type="cellIs" dxfId="291" priority="117" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="219" priority="117" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:J24 L24:M24">
-    <cfRule type="cellIs" dxfId="290" priority="118" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="218" priority="118" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:J24 L24:M24">
-    <cfRule type="cellIs" dxfId="289" priority="119" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="217" priority="119" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:J24 L24:M24">
-    <cfRule type="cellIs" dxfId="288" priority="120" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="216" priority="120" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="287" priority="114" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="215" priority="114" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="286" priority="115" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="214" priority="115" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="285" priority="116" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="213" priority="116" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L30">
-    <cfRule type="cellIs" dxfId="284" priority="101" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="212" priority="101" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I29 L29 G29 E29 C29">
-    <cfRule type="cellIs" dxfId="283" priority="109" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="211" priority="109" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29:M29">
-    <cfRule type="cellIs" dxfId="282" priority="110" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="210" priority="110" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29 F29 H29 J29 M29">
-    <cfRule type="cellIs" dxfId="281" priority="111" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="209" priority="111" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29:M29">
-    <cfRule type="cellIs" dxfId="280" priority="112" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="208" priority="112" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29:M29">
-    <cfRule type="cellIs" dxfId="279" priority="113" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="207" priority="113" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K29">
-    <cfRule type="cellIs" dxfId="278" priority="107" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="206" priority="107" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K29">
-    <cfRule type="cellIs" dxfId="277" priority="108" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="205" priority="108" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N29">
-    <cfRule type="cellIs" dxfId="276" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="204" priority="106" operator="equal">
       <formula>$B29</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="cellIs" dxfId="275" priority="105" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="203" priority="105" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30">
-    <cfRule type="cellIs" dxfId="274" priority="104" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="202" priority="104" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30">
-    <cfRule type="cellIs" dxfId="273" priority="103" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="201" priority="103" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="cellIs" dxfId="272" priority="102" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="200" priority="102" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14 I14 L14">
-    <cfRule type="cellIs" dxfId="255" priority="81" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="199" priority="81" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14:M14">
-    <cfRule type="cellIs" dxfId="254" priority="82" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="198" priority="82" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14:M14">
-    <cfRule type="cellIs" dxfId="253" priority="83" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="197" priority="83" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14:M14">
-    <cfRule type="cellIs" dxfId="252" priority="84" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="196" priority="84" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L22">
-    <cfRule type="cellIs" dxfId="223" priority="57" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="195" priority="57" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:M22">
-    <cfRule type="cellIs" dxfId="222" priority="58" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="194" priority="58" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:M22">
-    <cfRule type="cellIs" dxfId="221" priority="59" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="193" priority="59" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:M22">
-    <cfRule type="cellIs" dxfId="220" priority="60" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="192" priority="60" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6385,7 +5856,7 @@
   <dimension ref="A1:AF1004"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6612,11 +6083,11 @@
       </c>
     </row>
     <row r="6" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
       <c r="D6" s="22"/>
       <c r="E6" s="18"/>
       <c r="F6" s="22"/>
@@ -6653,7 +6124,9 @@
         <v>2.7777777777777776E-2</v>
       </c>
       <c r="C8" s="18"/>
-      <c r="D8" s="22"/>
+      <c r="D8" s="22">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="E8" s="18"/>
       <c r="F8" s="22"/>
       <c r="G8" s="18"/>
@@ -6665,7 +6138,7 @@
       <c r="M8" s="23"/>
       <c r="N8" s="6">
         <f t="shared" ref="N8:N13" si="0">SUM(C8:M8)</f>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="O8" s="11"/>
       <c r="P8" s="11"/>
@@ -6694,7 +6167,9 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="C9" s="25"/>
-      <c r="D9" s="26"/>
+      <c r="D9" s="26">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="E9" s="25"/>
       <c r="F9" s="26"/>
       <c r="G9" s="25"/>
@@ -6706,7 +6181,7 @@
       <c r="M9" s="27"/>
       <c r="N9" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="O9" s="11"/>
       <c r="P9" s="11"/>
@@ -6735,7 +6210,9 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="C10" s="25"/>
-      <c r="D10" s="26"/>
+      <c r="D10" s="26">
+        <v>6.25E-2</v>
+      </c>
       <c r="E10" s="25"/>
       <c r="F10" s="26"/>
       <c r="G10" s="25"/>
@@ -6747,7 +6224,7 @@
       <c r="M10" s="27"/>
       <c r="N10" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="O10" s="11"/>
       <c r="P10" s="11"/>
@@ -6776,7 +6253,9 @@
         <v>0.125</v>
       </c>
       <c r="C11" s="25"/>
-      <c r="D11" s="26"/>
+      <c r="D11" s="49">
+        <v>0.22222222222222221</v>
+      </c>
       <c r="E11" s="25"/>
       <c r="F11" s="26"/>
       <c r="G11" s="25"/>
@@ -6786,9 +6265,9 @@
       <c r="K11" s="26"/>
       <c r="L11" s="25"/>
       <c r="M11" s="27"/>
-      <c r="N11" s="6">
+      <c r="N11" s="48">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="O11" s="11"/>
       <c r="P11" s="11"/>
@@ -6892,14 +6371,14 @@
       <c r="AF13" s="11"/>
     </row>
     <row r="14" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
       <c r="G14" s="18"/>
       <c r="H14" s="22"/>
       <c r="I14" s="18"/>
@@ -7130,17 +6609,17 @@
       </c>
     </row>
     <row r="22" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="45"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="45"/>
-      <c r="G22" s="45"/>
-      <c r="H22" s="45"/>
-      <c r="I22" s="45"/>
+      <c r="B22" s="46"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="46"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="46"/>
       <c r="J22" s="22"/>
       <c r="K22" s="22"/>
       <c r="L22" s="18"/>
@@ -7461,21 +6940,21 @@
       <c r="AF30" s="11"/>
     </row>
     <row r="31" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="44" t="s">
+      <c r="A31" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="45"/>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="45"/>
-      <c r="K31" s="45"/>
-      <c r="L31" s="45"/>
-      <c r="M31" s="46"/>
+      <c r="B31" s="46"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="46"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="46"/>
+      <c r="I31" s="46"/>
+      <c r="J31" s="46"/>
+      <c r="K31" s="46"/>
+      <c r="L31" s="46"/>
+      <c r="M31" s="47"/>
     </row>
     <row r="32" spans="1:32" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="33" t="s">
@@ -7487,7 +6966,9 @@
       <c r="C32" s="31">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="D32" s="31"/>
+      <c r="D32" s="31">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="E32" s="31"/>
       <c r="F32" s="31"/>
       <c r="G32" s="31"/>
@@ -7499,7 +6980,7 @@
       <c r="M32" s="41"/>
       <c r="N32" s="6">
         <f>SUM(C32:M32)</f>
-        <v>1.3888888888888888E-2</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="O32" s="11"/>
       <c r="P32" s="11"/>
@@ -7531,7 +7012,7 @@
       </c>
       <c r="D33" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E33" s="6">
         <f t="shared" si="1"/>
@@ -7571,7 +7052,7 @@
       </c>
       <c r="N33" s="6">
         <f t="shared" si="1"/>
-        <v>0.33333333333333337</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="O33" s="11"/>
       <c r="P33" s="11"/>
@@ -7595,11 +7076,11 @@
     <row r="34" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M34" s="42">
         <f>SUM(C33:M33)</f>
-        <v>0.33333333333333337</v>
+        <v>0.66666666666666674</v>
       </c>
     </row>
     <row r="35" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F35" s="47" t="s">
+      <c r="F35" s="44" t="s">
         <v>28</v>
       </c>
     </row>
@@ -8598,482 +8079,482 @@
     <mergeCell ref="A31:M31"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:J3 C26:C27 I26:I27 L2:M3 E26:E27 G26:G27 L26:L27 L8:L13 I8:I13 G8:G13 E8:E13 C8:C13 L19 I19 G19 E19 C19 C4:C5 E4:E5 G4:G5 I4:I5 L4:L5 C23 C16:C17 E23 E16:E17 G23 G16:G17 I23 I16:I17 L23 L16:L17 I30 I32 L30 L32 G30 G32 E30 E32 C30 C32">
-    <cfRule type="cellIs" dxfId="183" priority="178" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="191" priority="178" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:M13 C25:M27 C19:M19 C2:M5 C23:M23 C16:M17 L32:M32 C30:M30 C32:J32">
-    <cfRule type="cellIs" dxfId="182" priority="179" operator="greaterThan">
+  <conditionalFormatting sqref="C8:M10 C25:M27 C19:M19 C2:M5 C23:M23 C16:M17 L32:M32 C30:M30 C32:J32 C12:M13 C11 E11:M11">
+    <cfRule type="cellIs" dxfId="190" priority="179" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L25 I25 G25 E25 C25">
-    <cfRule type="cellIs" dxfId="181" priority="180" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="189" priority="180" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:J25 L25:M25">
-    <cfRule type="cellIs" dxfId="180" priority="181" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="188" priority="181" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30 F30 H30 J30 M30">
-    <cfRule type="cellIs" dxfId="179" priority="182" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="187" priority="182" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:M13 C25:M27 C19:M19 C2:M5 C23:M23 C16:M17 L32:M32 C30:M30 C32:J32">
-    <cfRule type="cellIs" dxfId="178" priority="183" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8:M13 C25:M27 C19:M19 C2:M5 C23:M23 C16:M17 L32:M32 C30:M30 C32:J32">
-    <cfRule type="cellIs" dxfId="177" priority="184" operator="greaterThan">
+  <conditionalFormatting sqref="C8:M10 C25:M27 C19:M19 C2:M5 C23:M23 C16:M17 L32:M32 C30:M30 C32:J32 C12:M13 C11 E11:M11">
+    <cfRule type="cellIs" dxfId="186" priority="183" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8:M10 C25:M27 C19:M19 C2:M5 C23:M23 C16:M17 L32:M32 C30:M30 C32:J32 C12:M13 C11 E11:M11">
+    <cfRule type="cellIs" dxfId="185" priority="184" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K3">
-    <cfRule type="cellIs" dxfId="176" priority="174" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="184" priority="174" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K3 K9:K13 K26:K27 K17 K30">
-    <cfRule type="cellIs" dxfId="175" priority="175" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="183" priority="175" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K25">
-    <cfRule type="cellIs" dxfId="174" priority="176" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="182" priority="176" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="cellIs" dxfId="173" priority="177" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="181" priority="177" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3 N25:N27 N5 N19 N21 N8:N13 N15:N17 N23 N30 N32">
-    <cfRule type="cellIs" dxfId="172" priority="173" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="173" operator="equal">
       <formula>$B3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="cellIs" dxfId="171" priority="172" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="172" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33:M33">
-    <cfRule type="cellIs" dxfId="170" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="171" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32">
-    <cfRule type="cellIs" dxfId="169" priority="170" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="177" priority="170" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F32">
-    <cfRule type="cellIs" dxfId="168" priority="169" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="176" priority="169" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="cellIs" dxfId="167" priority="168" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="175" priority="168" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J32">
-    <cfRule type="cellIs" dxfId="166" priority="167" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="174" priority="167" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="165" priority="162" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="173" priority="162" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="164" priority="163" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="172" priority="163" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="163" priority="164" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="171" priority="164" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="162" priority="165" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="170" priority="165" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="161" priority="166" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="169" priority="166" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M32">
-    <cfRule type="cellIs" dxfId="160" priority="161" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="168" priority="161" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2">
-    <cfRule type="cellIs" dxfId="159" priority="160" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="160" operator="equal">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4">
-    <cfRule type="cellIs" dxfId="158" priority="159" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="159" operator="equal">
       <formula>$B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7 E7 G7 I7 L7">
-    <cfRule type="cellIs" dxfId="157" priority="155" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="165" priority="155" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:J7 L7:M7">
-    <cfRule type="cellIs" dxfId="156" priority="156" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="164" priority="156" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:J7 L7:M7">
-    <cfRule type="cellIs" dxfId="155" priority="157" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="163" priority="157" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:J7 L7:M7">
-    <cfRule type="cellIs" dxfId="154" priority="158" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="162" priority="158" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="153" priority="152" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="161" priority="152" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="152" priority="153" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="160" priority="153" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="151" priority="154" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="159" priority="154" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="150" priority="145" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="158" priority="145" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18 E18 G18 I18 L18">
-    <cfRule type="cellIs" dxfId="149" priority="148" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="157" priority="148" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:J18 L18:M18">
-    <cfRule type="cellIs" dxfId="148" priority="149" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="156" priority="149" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:J18 L18:M18">
-    <cfRule type="cellIs" dxfId="147" priority="150" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="155" priority="150" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:J18 L18:M18">
-    <cfRule type="cellIs" dxfId="146" priority="151" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="154" priority="151" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="145" priority="146" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="153" priority="146" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="144" priority="147" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="152" priority="147" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L21 I21 G21 E21 C21">
-    <cfRule type="cellIs" dxfId="143" priority="141" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="151" priority="141" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:M21">
-    <cfRule type="cellIs" dxfId="142" priority="142" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="150" priority="142" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:M21">
-    <cfRule type="cellIs" dxfId="141" priority="143" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="149" priority="143" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:M21">
-    <cfRule type="cellIs" dxfId="140" priority="144" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="148" priority="144" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21">
-    <cfRule type="cellIs" dxfId="139" priority="140" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="147" priority="140" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="cellIs" dxfId="138" priority="133" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="146" priority="133" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28">
-    <cfRule type="cellIs" dxfId="137" priority="121" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="145" priority="121" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20 E20 G20 I20 L20">
-    <cfRule type="cellIs" dxfId="136" priority="136" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="144" priority="136" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:J20 L20:M20">
-    <cfRule type="cellIs" dxfId="135" priority="137" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="143" priority="137" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:J20 L20:M20">
-    <cfRule type="cellIs" dxfId="134" priority="138" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="142" priority="138" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:J20 L20:M20">
-    <cfRule type="cellIs" dxfId="133" priority="139" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="141" priority="139" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="cellIs" dxfId="132" priority="134" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="140" priority="134" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="cellIs" dxfId="131" priority="135" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="139" priority="135" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L15 I15 G15 E15 C15">
-    <cfRule type="cellIs" dxfId="130" priority="129" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="138" priority="129" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:M15">
-    <cfRule type="cellIs" dxfId="129" priority="130" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="137" priority="130" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:M15">
-    <cfRule type="cellIs" dxfId="128" priority="131" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="136" priority="131" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:M15">
-    <cfRule type="cellIs" dxfId="127" priority="132" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="135" priority="132" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="cellIs" dxfId="126" priority="128" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="134" priority="128" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28 E28 G28 I28 L28">
-    <cfRule type="cellIs" dxfId="125" priority="124" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="133" priority="124" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:J28 L28:M28">
-    <cfRule type="cellIs" dxfId="124" priority="125" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="132" priority="125" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:J28 L28:M28">
-    <cfRule type="cellIs" dxfId="123" priority="126" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="131" priority="126" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:J28 L28:M28">
-    <cfRule type="cellIs" dxfId="122" priority="127" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="130" priority="127" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28">
-    <cfRule type="cellIs" dxfId="121" priority="122" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="129" priority="122" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28">
-    <cfRule type="cellIs" dxfId="120" priority="123" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="128" priority="123" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24 E24 G24 I24 L24">
-    <cfRule type="cellIs" dxfId="119" priority="117" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="127" priority="117" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:J24 L24:M24">
-    <cfRule type="cellIs" dxfId="118" priority="118" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="126" priority="118" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:J24 L24:M24">
-    <cfRule type="cellIs" dxfId="117" priority="119" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="125" priority="119" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:J24 L24:M24">
-    <cfRule type="cellIs" dxfId="116" priority="120" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="124" priority="120" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="115" priority="114" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="123" priority="114" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="114" priority="115" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="122" priority="115" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="113" priority="116" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="121" priority="116" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L30">
-    <cfRule type="cellIs" dxfId="112" priority="101" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="120" priority="101" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I29 L29 G29 E29 C29">
-    <cfRule type="cellIs" dxfId="111" priority="109" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="119" priority="109" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29:M29">
-    <cfRule type="cellIs" dxfId="110" priority="110" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="118" priority="110" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29 F29 H29 J29 M29">
-    <cfRule type="cellIs" dxfId="109" priority="111" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="117" priority="111" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29:M29">
-    <cfRule type="cellIs" dxfId="108" priority="112" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="116" priority="112" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29:M29">
-    <cfRule type="cellIs" dxfId="107" priority="113" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="115" priority="113" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K29">
-    <cfRule type="cellIs" dxfId="106" priority="107" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="114" priority="107" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K29">
-    <cfRule type="cellIs" dxfId="105" priority="108" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="113" priority="108" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N29">
-    <cfRule type="cellIs" dxfId="104" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="106" operator="equal">
       <formula>$B29</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="cellIs" dxfId="103" priority="105" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="111" priority="105" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30">
-    <cfRule type="cellIs" dxfId="102" priority="104" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="110" priority="104" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30">
-    <cfRule type="cellIs" dxfId="101" priority="103" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="109" priority="103" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="cellIs" dxfId="100" priority="102" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="108" priority="102" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6 G6 I6 L6">
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="107" priority="9" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:M6">
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="106" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:M6">
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="105" priority="11" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:M6">
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="104" priority="12" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14 I14 L14">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="103" priority="5" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14:M14">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="102" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14:M14">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="101" priority="7" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14:M14">
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="100" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L22">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="99" priority="1" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:M22">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="98" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:M22">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="97" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:M22">
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="96" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
docs: documentation du jour 3
</commit_message>
<xml_diff>
--- a/docs/plannification_TPI.xlsx
+++ b/docs/plannification_TPI.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17730"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17730" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionnel" sheetId="1" r:id="rId1"/>
@@ -549,6 +549,12 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="18" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -558,798 +564,12 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="18" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Insatisfaisant" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="284">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="188">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3091,8 +2311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3319,11 +2539,11 @@
       </c>
     </row>
     <row r="6" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
       <c r="D6" s="22"/>
       <c r="E6" s="18"/>
       <c r="F6" s="22"/>
@@ -3611,14 +2831,14 @@
       <c r="AF13" s="11"/>
     </row>
     <row r="14" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="46"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
       <c r="G14" s="18"/>
       <c r="H14" s="22"/>
       <c r="I14" s="18"/>
@@ -3863,17 +3083,17 @@
       </c>
     </row>
     <row r="22" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="45" t="s">
+      <c r="A22" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="46"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="46"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="46"/>
-      <c r="H22" s="46"/>
-      <c r="I22" s="46"/>
+      <c r="B22" s="48"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="48"/>
       <c r="J22" s="22"/>
       <c r="K22" s="22"/>
       <c r="L22" s="18"/>
@@ -4228,21 +3448,21 @@
       <c r="AF30" s="11"/>
     </row>
     <row r="31" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="45" t="s">
+      <c r="A31" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="46"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="46"/>
-      <c r="H31" s="46"/>
-      <c r="I31" s="46"/>
-      <c r="J31" s="46"/>
-      <c r="K31" s="46"/>
-      <c r="L31" s="46"/>
-      <c r="M31" s="47"/>
+      <c r="B31" s="48"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="48"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="48"/>
+      <c r="K31" s="48"/>
+      <c r="L31" s="48"/>
+      <c r="M31" s="49"/>
     </row>
     <row r="32" spans="1:32" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="33" t="s">
@@ -5387,462 +4607,462 @@
     <mergeCell ref="A14:F14"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:J3 C26:C27 I26:I27 L2:M3 E26:E27 G26:G27 L26:L27 L8:L13 I8:I13 G8:G13 E8:E13 C8:C13 L19 I19 G19 E19 C19 C4:C5 E4:E6 G4:G6 I4:I6 L4:L6 C23 C16:C17 E23 E16:E17 G23 G16:G17 I23 I16:I17 L23 L16:L17 I30 I32 L30 L32 G30 G32 E30 E32 C30 C32">
-    <cfRule type="cellIs" dxfId="283" priority="194" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="187" priority="194" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:M13 C25:M27 C19:M19 C2:M5 C23:M23 C16:M17 D6:M6 L32:M32 C30:M30 C32:J32">
-    <cfRule type="cellIs" dxfId="282" priority="195" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="186" priority="195" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L25 I25 G25 E25 C25">
-    <cfRule type="cellIs" dxfId="281" priority="196" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="185" priority="196" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:J25 L25:M25">
-    <cfRule type="cellIs" dxfId="280" priority="197" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="184" priority="197" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30 F30 H30 J30 M30">
-    <cfRule type="cellIs" dxfId="279" priority="198" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="183" priority="198" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:M13 C25:M27 C19:M19 C2:M5 C23:M23 C16:M17 D6:M6 L32:M32 C30:M30 C32:J32">
-    <cfRule type="cellIs" dxfId="278" priority="201" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="182" priority="201" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:M13 C25:M27 C19:M19 C2:M5 C23:M23 C16:M17 D6:M6 L32:M32 C30:M30 C32:J32">
-    <cfRule type="cellIs" dxfId="277" priority="202" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="181" priority="202" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K3">
-    <cfRule type="cellIs" dxfId="276" priority="186" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="180" priority="186" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K3 K9:K13 K26:K27 K17 K30">
-    <cfRule type="cellIs" dxfId="275" priority="187" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="179" priority="187" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K25">
-    <cfRule type="cellIs" dxfId="274" priority="188" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="178" priority="188" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="cellIs" dxfId="273" priority="189" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="177" priority="189" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3 N25:N27 N5 N19 N21 N8:N13 N15:N17 N23 N30 N32">
-    <cfRule type="cellIs" dxfId="272" priority="184" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="184" operator="equal">
       <formula>$B3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="cellIs" dxfId="271" priority="181" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="181" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33:M33">
-    <cfRule type="cellIs" dxfId="270" priority="180" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="180" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32">
-    <cfRule type="cellIs" dxfId="269" priority="177" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="173" priority="177" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F32">
-    <cfRule type="cellIs" dxfId="268" priority="176" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="172" priority="176" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="cellIs" dxfId="267" priority="175" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="171" priority="175" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J32">
-    <cfRule type="cellIs" dxfId="266" priority="174" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="170" priority="174" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="265" priority="169" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="169" priority="169" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="264" priority="170" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="168" priority="170" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="263" priority="171" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="167" priority="171" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="262" priority="172" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="166" priority="172" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="261" priority="173" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="165" priority="173" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M32">
-    <cfRule type="cellIs" dxfId="260" priority="168" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="164" priority="168" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2">
-    <cfRule type="cellIs" dxfId="259" priority="167" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="167" operator="equal">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4">
-    <cfRule type="cellIs" dxfId="258" priority="166" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="166" operator="equal">
       <formula>$B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7 E7 G7 I7 L7">
-    <cfRule type="cellIs" dxfId="257" priority="162" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="161" priority="162" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:J7 L7:M7">
-    <cfRule type="cellIs" dxfId="256" priority="163" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="160" priority="163" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:J7 L7:M7">
-    <cfRule type="cellIs" dxfId="255" priority="164" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="159" priority="164" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:J7 L7:M7">
-    <cfRule type="cellIs" dxfId="254" priority="165" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="158" priority="165" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="253" priority="159" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="157" priority="159" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="252" priority="160" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="156" priority="160" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="251" priority="161" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="155" priority="161" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="250" priority="152" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="154" priority="152" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18 E18 G18 I18 L18">
-    <cfRule type="cellIs" dxfId="249" priority="155" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="153" priority="155" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:J18 L18:M18">
-    <cfRule type="cellIs" dxfId="248" priority="156" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="152" priority="156" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:J18 L18:M18">
-    <cfRule type="cellIs" dxfId="247" priority="157" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="151" priority="157" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:J18 L18:M18">
-    <cfRule type="cellIs" dxfId="246" priority="158" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="150" priority="158" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="245" priority="153" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="149" priority="153" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="244" priority="154" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="148" priority="154" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L21 I21 G21 E21 C21">
-    <cfRule type="cellIs" dxfId="243" priority="143" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="147" priority="143" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:M21">
-    <cfRule type="cellIs" dxfId="242" priority="144" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="146" priority="144" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:M21">
-    <cfRule type="cellIs" dxfId="241" priority="145" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="145" priority="145" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:M21">
-    <cfRule type="cellIs" dxfId="240" priority="146" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="144" priority="146" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21">
-    <cfRule type="cellIs" dxfId="239" priority="142" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="143" priority="142" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="cellIs" dxfId="238" priority="134" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="142" priority="134" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28">
-    <cfRule type="cellIs" dxfId="237" priority="121" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="141" priority="121" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20 E20 G20 I20 L20">
-    <cfRule type="cellIs" dxfId="236" priority="137" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="140" priority="137" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:J20 L20:M20">
-    <cfRule type="cellIs" dxfId="235" priority="138" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="139" priority="138" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:J20 L20:M20">
-    <cfRule type="cellIs" dxfId="234" priority="139" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="138" priority="139" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:J20 L20:M20">
-    <cfRule type="cellIs" dxfId="233" priority="140" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="137" priority="140" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="cellIs" dxfId="232" priority="135" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="136" priority="135" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="cellIs" dxfId="231" priority="136" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="135" priority="136" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L15 I15 G15 E15 C15">
-    <cfRule type="cellIs" dxfId="230" priority="130" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="134" priority="130" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:M15">
-    <cfRule type="cellIs" dxfId="229" priority="131" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="133" priority="131" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:M15">
-    <cfRule type="cellIs" dxfId="228" priority="132" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="132" priority="132" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:M15">
-    <cfRule type="cellIs" dxfId="227" priority="133" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="131" priority="133" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="cellIs" dxfId="226" priority="129" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="130" priority="129" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28 E28 G28 I28 L28">
-    <cfRule type="cellIs" dxfId="225" priority="124" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="129" priority="124" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:J28 L28:M28">
-    <cfRule type="cellIs" dxfId="224" priority="125" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="128" priority="125" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:J28 L28:M28">
-    <cfRule type="cellIs" dxfId="223" priority="126" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="127" priority="126" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:J28 L28:M28">
-    <cfRule type="cellIs" dxfId="222" priority="127" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="126" priority="127" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28">
-    <cfRule type="cellIs" dxfId="221" priority="122" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="125" priority="122" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28">
-    <cfRule type="cellIs" dxfId="220" priority="123" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="124" priority="123" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24 E24 G24 I24 L24">
-    <cfRule type="cellIs" dxfId="219" priority="117" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="123" priority="117" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:J24 L24:M24">
-    <cfRule type="cellIs" dxfId="218" priority="118" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="122" priority="118" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:J24 L24:M24">
-    <cfRule type="cellIs" dxfId="217" priority="119" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="121" priority="119" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:J24 L24:M24">
-    <cfRule type="cellIs" dxfId="216" priority="120" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="120" priority="120" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="215" priority="114" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="119" priority="114" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="214" priority="115" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="118" priority="115" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="213" priority="116" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="117" priority="116" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L30">
-    <cfRule type="cellIs" dxfId="212" priority="101" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="116" priority="101" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I29 L29 G29 E29 C29">
-    <cfRule type="cellIs" dxfId="211" priority="109" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="115" priority="109" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29:M29">
-    <cfRule type="cellIs" dxfId="210" priority="110" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="114" priority="110" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29 F29 H29 J29 M29">
-    <cfRule type="cellIs" dxfId="209" priority="111" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="113" priority="111" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29:M29">
-    <cfRule type="cellIs" dxfId="208" priority="112" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="112" priority="112" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29:M29">
-    <cfRule type="cellIs" dxfId="207" priority="113" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="111" priority="113" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K29">
-    <cfRule type="cellIs" dxfId="206" priority="107" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="110" priority="107" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K29">
-    <cfRule type="cellIs" dxfId="205" priority="108" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="109" priority="108" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N29">
-    <cfRule type="cellIs" dxfId="204" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="106" operator="equal">
       <formula>$B29</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="cellIs" dxfId="203" priority="105" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="107" priority="105" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30">
-    <cfRule type="cellIs" dxfId="202" priority="104" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="106" priority="104" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30">
-    <cfRule type="cellIs" dxfId="201" priority="103" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="105" priority="103" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="cellIs" dxfId="200" priority="102" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="104" priority="102" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14 I14 L14">
-    <cfRule type="cellIs" dxfId="199" priority="81" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="103" priority="81" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14:M14">
-    <cfRule type="cellIs" dxfId="198" priority="82" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="102" priority="82" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14:M14">
-    <cfRule type="cellIs" dxfId="197" priority="83" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="101" priority="83" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14:M14">
-    <cfRule type="cellIs" dxfId="196" priority="84" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="100" priority="84" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L22">
-    <cfRule type="cellIs" dxfId="195" priority="57" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="99" priority="57" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:M22">
-    <cfRule type="cellIs" dxfId="194" priority="58" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="98" priority="58" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:M22">
-    <cfRule type="cellIs" dxfId="193" priority="59" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="97" priority="59" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:M22">
-    <cfRule type="cellIs" dxfId="192" priority="60" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="96" priority="60" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5855,8 +5075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF1004"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P36" sqref="P36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6083,11 +5303,11 @@
       </c>
     </row>
     <row r="6" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
       <c r="D6" s="22"/>
       <c r="E6" s="18"/>
       <c r="F6" s="22"/>
@@ -6253,7 +5473,7 @@
         <v>0.125</v>
       </c>
       <c r="C11" s="25"/>
-      <c r="D11" s="49">
+      <c r="D11" s="46">
         <v>0.22222222222222221</v>
       </c>
       <c r="E11" s="25"/>
@@ -6265,7 +5485,7 @@
       <c r="K11" s="26"/>
       <c r="L11" s="25"/>
       <c r="M11" s="27"/>
-      <c r="N11" s="48">
+      <c r="N11" s="45">
         <f t="shared" si="0"/>
         <v>0.22222222222222221</v>
       </c>
@@ -6297,7 +5517,9 @@
       </c>
       <c r="C12" s="25"/>
       <c r="D12" s="26"/>
-      <c r="E12" s="25"/>
+      <c r="E12" s="25">
+        <v>0.27083333333333331</v>
+      </c>
       <c r="F12" s="26"/>
       <c r="G12" s="25"/>
       <c r="H12" s="26"/>
@@ -6308,7 +5530,7 @@
       <c r="M12" s="27"/>
       <c r="N12" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.27083333333333331</v>
       </c>
       <c r="O12" s="11"/>
       <c r="P12" s="11"/>
@@ -6371,14 +5593,14 @@
       <c r="AF13" s="11"/>
     </row>
     <row r="14" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="46"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
       <c r="G14" s="18"/>
       <c r="H14" s="22"/>
       <c r="I14" s="18"/>
@@ -6609,17 +5831,17 @@
       </c>
     </row>
     <row r="22" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="45" t="s">
+      <c r="A22" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="46"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="46"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="46"/>
-      <c r="H22" s="46"/>
-      <c r="I22" s="46"/>
+      <c r="B22" s="48"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="48"/>
       <c r="J22" s="22"/>
       <c r="K22" s="22"/>
       <c r="L22" s="18"/>
@@ -6907,7 +6129,9 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
+      <c r="E30" s="25">
+        <v>4.8611111111111112E-2</v>
+      </c>
       <c r="F30" s="25"/>
       <c r="G30" s="25"/>
       <c r="H30" s="25"/>
@@ -6918,7 +6142,7 @@
       <c r="M30" s="40"/>
       <c r="N30" s="6">
         <f>SUM(C30:M30)</f>
-        <v>4.1666666666666664E-2</v>
+        <v>9.0277777777777776E-2</v>
       </c>
       <c r="O30" s="11"/>
       <c r="P30" s="11"/>
@@ -6940,21 +6164,21 @@
       <c r="AF30" s="11"/>
     </row>
     <row r="31" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="45" t="s">
+      <c r="A31" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="46"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="46"/>
-      <c r="H31" s="46"/>
-      <c r="I31" s="46"/>
-      <c r="J31" s="46"/>
-      <c r="K31" s="46"/>
-      <c r="L31" s="46"/>
-      <c r="M31" s="47"/>
+      <c r="B31" s="48"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="48"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="48"/>
+      <c r="K31" s="48"/>
+      <c r="L31" s="48"/>
+      <c r="M31" s="49"/>
     </row>
     <row r="32" spans="1:32" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="33" t="s">
@@ -6969,7 +6193,9 @@
       <c r="D32" s="31">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="E32" s="31"/>
+      <c r="E32" s="31">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="F32" s="31"/>
       <c r="G32" s="31"/>
       <c r="H32" s="31"/>
@@ -6980,7 +6206,7 @@
       <c r="M32" s="41"/>
       <c r="N32" s="6">
         <f>SUM(C32:M32)</f>
-        <v>2.7777777777777776E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="O32" s="11"/>
       <c r="P32" s="11"/>
@@ -7016,7 +6242,7 @@
       </c>
       <c r="E33" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F33" s="6">
         <f t="shared" si="1"/>
@@ -7052,7 +6278,7 @@
       </c>
       <c r="N33" s="6">
         <f t="shared" si="1"/>
-        <v>0.66666666666666663</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="O33" s="11"/>
       <c r="P33" s="11"/>
@@ -7076,7 +6302,7 @@
     <row r="34" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M34" s="42">
         <f>SUM(C33:M33)</f>
-        <v>0.66666666666666674</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -8079,482 +7305,482 @@
     <mergeCell ref="A31:M31"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:J3 C26:C27 I26:I27 L2:M3 E26:E27 G26:G27 L26:L27 L8:L13 I8:I13 G8:G13 E8:E13 C8:C13 L19 I19 G19 E19 C19 C4:C5 E4:E5 G4:G5 I4:I5 L4:L5 C23 C16:C17 E23 E16:E17 G23 G16:G17 I23 I16:I17 L23 L16:L17 I30 I32 L30 L32 G30 G32 E30 E32 C30 C32">
-    <cfRule type="cellIs" dxfId="191" priority="178" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="95" priority="178" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:M10 C25:M27 C19:M19 C2:M5 C23:M23 C16:M17 L32:M32 C30:M30 C32:J32 C12:M13 C11 E11:M11">
-    <cfRule type="cellIs" dxfId="190" priority="179" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="94" priority="179" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L25 I25 G25 E25 C25">
-    <cfRule type="cellIs" dxfId="189" priority="180" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="93" priority="180" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:J25 L25:M25">
-    <cfRule type="cellIs" dxfId="188" priority="181" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="92" priority="181" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30 F30 H30 J30 M30">
-    <cfRule type="cellIs" dxfId="187" priority="182" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="91" priority="182" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:M10 C25:M27 C19:M19 C2:M5 C23:M23 C16:M17 L32:M32 C30:M30 C32:J32 C12:M13 C11 E11:M11">
-    <cfRule type="cellIs" dxfId="186" priority="183" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="90" priority="183" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:M10 C25:M27 C19:M19 C2:M5 C23:M23 C16:M17 L32:M32 C30:M30 C32:J32 C12:M13 C11 E11:M11">
-    <cfRule type="cellIs" dxfId="185" priority="184" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="89" priority="184" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K3">
-    <cfRule type="cellIs" dxfId="184" priority="174" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="88" priority="174" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K3 K9:K13 K26:K27 K17 K30">
-    <cfRule type="cellIs" dxfId="183" priority="175" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="87" priority="175" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K25">
-    <cfRule type="cellIs" dxfId="182" priority="176" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="86" priority="176" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="cellIs" dxfId="181" priority="177" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="85" priority="177" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3 N25:N27 N5 N19 N21 N8:N13 N15:N17 N23 N30 N32">
-    <cfRule type="cellIs" dxfId="180" priority="173" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="173" operator="equal">
       <formula>$B3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="cellIs" dxfId="179" priority="172" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="172" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33:M33">
-    <cfRule type="cellIs" dxfId="178" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="171" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32">
-    <cfRule type="cellIs" dxfId="177" priority="170" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="81" priority="170" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F32">
-    <cfRule type="cellIs" dxfId="176" priority="169" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="80" priority="169" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="cellIs" dxfId="175" priority="168" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="79" priority="168" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J32">
-    <cfRule type="cellIs" dxfId="174" priority="167" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="78" priority="167" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="173" priority="162" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="77" priority="162" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="172" priority="163" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="76" priority="163" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="171" priority="164" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="75" priority="164" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="170" priority="165" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="74" priority="165" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="169" priority="166" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="73" priority="166" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M32">
-    <cfRule type="cellIs" dxfId="168" priority="161" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="72" priority="161" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2">
-    <cfRule type="cellIs" dxfId="167" priority="160" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="160" operator="equal">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4">
-    <cfRule type="cellIs" dxfId="166" priority="159" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="159" operator="equal">
       <formula>$B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7 E7 G7 I7 L7">
-    <cfRule type="cellIs" dxfId="165" priority="155" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="69" priority="155" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:J7 L7:M7">
-    <cfRule type="cellIs" dxfId="164" priority="156" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="68" priority="156" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:J7 L7:M7">
-    <cfRule type="cellIs" dxfId="163" priority="157" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="67" priority="157" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:J7 L7:M7">
-    <cfRule type="cellIs" dxfId="162" priority="158" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="66" priority="158" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="161" priority="152" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="65" priority="152" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="160" priority="153" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="64" priority="153" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="159" priority="154" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="63" priority="154" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="158" priority="145" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="62" priority="145" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18 E18 G18 I18 L18">
-    <cfRule type="cellIs" dxfId="157" priority="148" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="61" priority="148" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:J18 L18:M18">
-    <cfRule type="cellIs" dxfId="156" priority="149" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="60" priority="149" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:J18 L18:M18">
-    <cfRule type="cellIs" dxfId="155" priority="150" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="59" priority="150" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:J18 L18:M18">
-    <cfRule type="cellIs" dxfId="154" priority="151" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="58" priority="151" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="153" priority="146" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="57" priority="146" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="152" priority="147" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="56" priority="147" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L21 I21 G21 E21 C21">
-    <cfRule type="cellIs" dxfId="151" priority="141" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="55" priority="141" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:M21">
-    <cfRule type="cellIs" dxfId="150" priority="142" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="54" priority="142" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:M21">
-    <cfRule type="cellIs" dxfId="149" priority="143" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="53" priority="143" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:M21">
-    <cfRule type="cellIs" dxfId="148" priority="144" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="52" priority="144" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21">
-    <cfRule type="cellIs" dxfId="147" priority="140" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="51" priority="140" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="cellIs" dxfId="146" priority="133" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="50" priority="133" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28">
-    <cfRule type="cellIs" dxfId="145" priority="121" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="49" priority="121" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20 E20 G20 I20 L20">
-    <cfRule type="cellIs" dxfId="144" priority="136" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="48" priority="136" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:J20 L20:M20">
-    <cfRule type="cellIs" dxfId="143" priority="137" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="47" priority="137" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:J20 L20:M20">
-    <cfRule type="cellIs" dxfId="142" priority="138" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="138" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:J20 L20:M20">
-    <cfRule type="cellIs" dxfId="141" priority="139" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="139" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="cellIs" dxfId="140" priority="134" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="44" priority="134" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="cellIs" dxfId="139" priority="135" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="135" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L15 I15 G15 E15 C15">
-    <cfRule type="cellIs" dxfId="138" priority="129" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="129" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:M15">
-    <cfRule type="cellIs" dxfId="137" priority="130" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="130" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:M15">
-    <cfRule type="cellIs" dxfId="136" priority="131" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="40" priority="131" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:M15">
-    <cfRule type="cellIs" dxfId="135" priority="132" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="132" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="cellIs" dxfId="134" priority="128" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="38" priority="128" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28 E28 G28 I28 L28">
-    <cfRule type="cellIs" dxfId="133" priority="124" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="124" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:J28 L28:M28">
-    <cfRule type="cellIs" dxfId="132" priority="125" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="125" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:J28 L28:M28">
-    <cfRule type="cellIs" dxfId="131" priority="126" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="126" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:J28 L28:M28">
-    <cfRule type="cellIs" dxfId="130" priority="127" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="127" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28">
-    <cfRule type="cellIs" dxfId="129" priority="122" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="122" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28">
-    <cfRule type="cellIs" dxfId="128" priority="123" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="123" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24 E24 G24 I24 L24">
-    <cfRule type="cellIs" dxfId="127" priority="117" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="117" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:J24 L24:M24">
-    <cfRule type="cellIs" dxfId="126" priority="118" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="118" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:J24 L24:M24">
-    <cfRule type="cellIs" dxfId="125" priority="119" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="119" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:J24 L24:M24">
-    <cfRule type="cellIs" dxfId="124" priority="120" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="120" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="123" priority="114" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="114" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="122" priority="115" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="115" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="121" priority="116" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="116" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L30">
-    <cfRule type="cellIs" dxfId="120" priority="101" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="101" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I29 L29 G29 E29 C29">
-    <cfRule type="cellIs" dxfId="119" priority="109" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="109" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29:M29">
-    <cfRule type="cellIs" dxfId="118" priority="110" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="110" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29 F29 H29 J29 M29">
-    <cfRule type="cellIs" dxfId="117" priority="111" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="111" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29:M29">
-    <cfRule type="cellIs" dxfId="116" priority="112" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="112" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29:M29">
-    <cfRule type="cellIs" dxfId="115" priority="113" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="113" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K29">
-    <cfRule type="cellIs" dxfId="114" priority="107" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="107" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K29">
-    <cfRule type="cellIs" dxfId="113" priority="108" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="108" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N29">
-    <cfRule type="cellIs" dxfId="112" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="106" operator="equal">
       <formula>$B29</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="cellIs" dxfId="111" priority="105" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="105" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30">
-    <cfRule type="cellIs" dxfId="110" priority="104" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="104" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30">
-    <cfRule type="cellIs" dxfId="109" priority="103" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="103" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="cellIs" dxfId="108" priority="102" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="102" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6 G6 I6 L6">
-    <cfRule type="cellIs" dxfId="107" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:M6">
-    <cfRule type="cellIs" dxfId="106" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:M6">
-    <cfRule type="cellIs" dxfId="105" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:M6">
-    <cfRule type="cellIs" dxfId="104" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14 I14 L14">
-    <cfRule type="cellIs" dxfId="103" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14:M14">
-    <cfRule type="cellIs" dxfId="102" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14:M14">
-    <cfRule type="cellIs" dxfId="101" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14:M14">
-    <cfRule type="cellIs" dxfId="100" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L22">
-    <cfRule type="cellIs" dxfId="99" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:M22">
-    <cfRule type="cellIs" dxfId="98" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:M22">
-    <cfRule type="cellIs" dxfId="97" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:M22">
-    <cfRule type="cellIs" dxfId="96" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
docs: documentation du jour 4
</commit_message>
<xml_diff>
--- a/docs/plannification_TPI.xlsx
+++ b/docs/plannification_TPI.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="37">
   <si>
     <t>Tâches à réaliser</t>
   </si>
@@ -140,6 +140,12 @@
   </si>
   <si>
     <t>Musique choisie joué en boucle dans la page jeu</t>
+  </si>
+  <si>
+    <t>Création du fichier de configuration</t>
+  </si>
+  <si>
+    <t>Temps prévu</t>
   </si>
 </sst>
 </file>
@@ -2312,7 +2318,7 @@
   <dimension ref="A1:AF1004"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5073,10 +5079,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF1004"/>
+  <dimension ref="A1:AF1005"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P36" sqref="P36"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5091,7 +5097,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="C1" s="9">
         <v>45406</v>
@@ -5561,7 +5567,9 @@
       <c r="C13" s="28"/>
       <c r="D13" s="26"/>
       <c r="E13" s="28"/>
-      <c r="F13" s="26"/>
+      <c r="F13" s="26">
+        <v>6.25E-2</v>
+      </c>
       <c r="G13" s="28"/>
       <c r="H13" s="26"/>
       <c r="I13" s="28"/>
@@ -5571,7 +5579,7 @@
       <c r="M13" s="27"/>
       <c r="N13" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="O13" s="11"/>
       <c r="P13" s="11"/>
@@ -5637,7 +5645,9 @@
       <c r="C15" s="28"/>
       <c r="D15" s="26"/>
       <c r="E15" s="28"/>
-      <c r="F15" s="26"/>
+      <c r="F15" s="26">
+        <v>0.19444444444444445</v>
+      </c>
       <c r="G15" s="25"/>
       <c r="H15" s="26"/>
       <c r="I15" s="28"/>
@@ -5647,7 +5657,7 @@
       <c r="M15" s="27"/>
       <c r="N15" s="6">
         <f>SUM(C15:M15)</f>
-        <v>0</v>
+        <v>0.19444444444444445</v>
       </c>
       <c r="O15" s="11"/>
       <c r="P15" s="11"/>
@@ -5670,84 +5680,92 @@
     </row>
     <row r="16" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B16" s="17">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="18"/>
+        <v>0</v>
+      </c>
+      <c r="C16" s="28"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="26">
+        <v>6.25E-2</v>
+      </c>
+      <c r="G16" s="25"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="28"/>
       <c r="M16" s="23"/>
       <c r="N16" s="6">
         <f>SUM(C16:M16)</f>
-        <v>0</v>
-      </c>
+        <v>6.25E-2</v>
+      </c>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="11"/>
+      <c r="U16" s="11"/>
+      <c r="V16" s="11"/>
+      <c r="W16" s="11"/>
+      <c r="X16" s="11"/>
+      <c r="Y16" s="11"/>
+      <c r="Z16" s="11"/>
+      <c r="AA16" s="11"/>
+      <c r="AB16" s="11"/>
+      <c r="AC16" s="11"/>
+      <c r="AD16" s="11"/>
+      <c r="AE16" s="11"/>
+      <c r="AF16" s="11"/>
     </row>
     <row r="17" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="24">
+        <v>33</v>
+      </c>
+      <c r="B17" s="17">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="27"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="23"/>
       <c r="N17" s="6">
         <f>SUM(C17:M17)</f>
         <v>0</v>
       </c>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="11"/>
-      <c r="R17" s="11"/>
-      <c r="S17" s="11"/>
-      <c r="T17" s="11"/>
-      <c r="U17" s="11"/>
-      <c r="V17" s="11"/>
-      <c r="W17" s="11"/>
-      <c r="X17" s="11"/>
-      <c r="Y17" s="11"/>
-      <c r="Z17" s="11"/>
-      <c r="AA17" s="11"/>
-      <c r="AB17" s="11"/>
-      <c r="AC17" s="11"/>
-      <c r="AD17" s="11"/>
-      <c r="AE17" s="11"/>
-      <c r="AF17" s="11"/>
     </row>
     <row r="18" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="5"/>
+      <c r="A18" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="24">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C18" s="28"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="6">
+        <f>SUM(C18:M18)</f>
+        <v>0</v>
+      </c>
       <c r="O18" s="11"/>
       <c r="P18" s="11"/>
       <c r="Q18" s="11"/>
@@ -5768,142 +5786,142 @@
       <c r="AF18" s="11"/>
     </row>
     <row r="19" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="5"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="11"/>
+      <c r="V19" s="11"/>
+      <c r="W19" s="11"/>
+      <c r="X19" s="11"/>
+      <c r="Y19" s="11"/>
+      <c r="Z19" s="11"/>
+      <c r="AA19" s="11"/>
+      <c r="AB19" s="11"/>
+      <c r="AC19" s="11"/>
+      <c r="AD19" s="11"/>
+      <c r="AE19" s="11"/>
+      <c r="AF19" s="11"/>
+    </row>
+    <row r="20" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="24">
+      <c r="B20" s="24">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C19" s="28"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="27"/>
-      <c r="N19" s="6">
-        <f>SUM(C19:M19)</f>
+      <c r="C20" s="28"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="6">
+        <f>SUM(C20:M20)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="34" t="s">
+    <row r="21" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="5"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="5"/>
     </row>
-    <row r="21" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="35" t="s">
+    <row r="22" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="24">
+      <c r="B22" s="24">
         <v>0.2638888888888889</v>
       </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="27"/>
-      <c r="N21" s="6">
-        <f>SUM(C21:M21)</f>
+      <c r="C22" s="28"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="27"/>
+      <c r="N22" s="6">
+        <f>SUM(C22:M22)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="47" t="s">
+    <row r="23" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="48"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="48"/>
-      <c r="E22" s="48"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="48"/>
-      <c r="H22" s="48"/>
-      <c r="I22" s="48"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="23"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="23"/>
     </row>
-    <row r="23" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="35" t="s">
+    <row r="24" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="17">
+      <c r="B24" s="17">
         <v>0.2986111111111111</v>
       </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="28"/>
-      <c r="M23" s="23"/>
-      <c r="N23" s="6">
-        <f>SUM(C23:M23)</f>
+      <c r="C24" s="28"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="6">
+        <f>SUM(C24:M24)</f>
         <v>0</v>
       </c>
-      <c r="O23" s="11"/>
-      <c r="P23" s="11"/>
-      <c r="Q23" s="11"/>
-      <c r="R23" s="11"/>
-      <c r="S23" s="11"/>
-      <c r="T23" s="11"/>
-      <c r="U23" s="11"/>
-      <c r="V23" s="11"/>
-      <c r="W23" s="11"/>
-      <c r="X23" s="11"/>
-      <c r="Y23" s="11"/>
-      <c r="Z23" s="11"/>
-      <c r="AA23" s="11"/>
-      <c r="AB23" s="11"/>
-      <c r="AC23" s="11"/>
-      <c r="AD23" s="11"/>
-      <c r="AE23" s="11"/>
-      <c r="AF23" s="11"/>
-    </row>
-    <row r="24" spans="1:32" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="5"/>
       <c r="O24" s="11"/>
       <c r="P24" s="11"/>
       <c r="Q24" s="11"/>
@@ -5923,26 +5941,22 @@
       <c r="AE24" s="11"/>
       <c r="AF24" s="11"/>
     </row>
-    <row r="25" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="24"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="25"/>
-      <c r="M25" s="27"/>
-      <c r="N25" s="6">
-        <f>SUM(C25:M25)</f>
-        <v>0</v>
-      </c>
+    <row r="25" spans="1:32" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="5"/>
       <c r="O25" s="11"/>
       <c r="P25" s="11"/>
       <c r="Q25" s="11"/>
@@ -5964,7 +5978,7 @@
     </row>
     <row r="26" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="35" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B26" s="24"/>
       <c r="C26" s="25"/>
@@ -6003,14 +6017,14 @@
     </row>
     <row r="27" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="35" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B27" s="24"/>
-      <c r="C27" s="28"/>
+      <c r="C27" s="25"/>
       <c r="D27" s="26"/>
-      <c r="E27" s="28"/>
+      <c r="E27" s="25"/>
       <c r="F27" s="26"/>
-      <c r="G27" s="28"/>
+      <c r="G27" s="25"/>
       <c r="H27" s="26"/>
       <c r="I27" s="25"/>
       <c r="J27" s="26"/>
@@ -6040,22 +6054,26 @@
       <c r="AE27" s="11"/>
       <c r="AF27" s="11"/>
     </row>
-    <row r="28" spans="1:32" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="5"/>
+    <row r="28" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="24"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="26"/>
+      <c r="K28" s="26"/>
+      <c r="L28" s="25"/>
+      <c r="M28" s="27"/>
+      <c r="N28" s="6">
+        <f>SUM(C28:M28)</f>
+        <v>0</v>
+      </c>
       <c r="O28" s="11"/>
       <c r="P28" s="11"/>
       <c r="Q28" s="11"/>
@@ -6075,30 +6093,22 @@
       <c r="AE28" s="11"/>
       <c r="AF28" s="11"/>
     </row>
-    <row r="29" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="B29" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="C29" s="25">
-        <v>0.10416666666666667</v>
-      </c>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
-      <c r="K29" s="25"/>
-      <c r="L29" s="25"/>
-      <c r="M29" s="29"/>
-      <c r="N29" s="6">
-        <f>SUM(C29:M29)</f>
-        <v>0.10416666666666667</v>
-      </c>
+    <row r="29" spans="1:32" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="5"/>
       <c r="O29" s="11"/>
       <c r="P29" s="11"/>
       <c r="Q29" s="11"/>
@@ -6119,30 +6129,28 @@
       <c r="AF29" s="11"/>
     </row>
     <row r="30" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="32" t="s">
-        <v>4</v>
+      <c r="A30" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="B30" s="24">
-        <v>1.0416666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="C30" s="25">
-        <v>4.1666666666666664E-2</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="D30" s="25"/>
-      <c r="E30" s="25">
-        <v>4.8611111111111112E-2</v>
-      </c>
+      <c r="E30" s="25"/>
       <c r="F30" s="25"/>
       <c r="G30" s="25"/>
       <c r="H30" s="25"/>
       <c r="I30" s="25"/>
       <c r="J30" s="25"/>
       <c r="K30" s="25"/>
-      <c r="L30" s="39"/>
-      <c r="M30" s="40"/>
+      <c r="L30" s="25"/>
+      <c r="M30" s="29"/>
       <c r="N30" s="6">
         <f>SUM(C30:M30)</f>
-        <v>9.0277777777777776E-2</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="O30" s="11"/>
       <c r="P30" s="11"/>
@@ -6163,122 +6171,97 @@
       <c r="AE30" s="11"/>
       <c r="AF30" s="11"/>
     </row>
-    <row r="31" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="47" t="s">
+    <row r="31" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="24">
+        <v>1.0416666666666667</v>
+      </c>
+      <c r="C31" s="25">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25">
+        <v>4.8611111111111112E-2</v>
+      </c>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="25"/>
+      <c r="J31" s="25"/>
+      <c r="K31" s="25"/>
+      <c r="L31" s="39"/>
+      <c r="M31" s="40"/>
+      <c r="N31" s="6">
+        <f>SUM(C31:M31)</f>
+        <v>9.0277777777777776E-2</v>
+      </c>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="11"/>
+      <c r="R31" s="11"/>
+      <c r="S31" s="11"/>
+      <c r="T31" s="11"/>
+      <c r="U31" s="11"/>
+      <c r="V31" s="11"/>
+      <c r="W31" s="11"/>
+      <c r="X31" s="11"/>
+      <c r="Y31" s="11"/>
+      <c r="Z31" s="11"/>
+      <c r="AA31" s="11"/>
+      <c r="AB31" s="11"/>
+      <c r="AC31" s="11"/>
+      <c r="AD31" s="11"/>
+      <c r="AE31" s="11"/>
+      <c r="AF31" s="11"/>
+    </row>
+    <row r="32" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="48"/>
-      <c r="C31" s="48"/>
-      <c r="D31" s="48"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="48"/>
-      <c r="G31" s="48"/>
-      <c r="H31" s="48"/>
-      <c r="I31" s="48"/>
-      <c r="J31" s="48"/>
-      <c r="K31" s="48"/>
-      <c r="L31" s="48"/>
-      <c r="M31" s="49"/>
+      <c r="B32" s="48"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="48"/>
+      <c r="E32" s="48"/>
+      <c r="F32" s="48"/>
+      <c r="G32" s="48"/>
+      <c r="H32" s="48"/>
+      <c r="I32" s="48"/>
+      <c r="J32" s="48"/>
+      <c r="K32" s="48"/>
+      <c r="L32" s="48"/>
+      <c r="M32" s="49"/>
     </row>
-    <row r="32" spans="1:32" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="33" t="s">
+    <row r="33" spans="1:32" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="30">
+      <c r="B33" s="30">
         <v>0.15277777777777776</v>
       </c>
-      <c r="C32" s="31">
+      <c r="C33" s="31">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="D32" s="31">
+      <c r="D33" s="31">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="E32" s="31">
+      <c r="E33" s="31">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="31"/>
-      <c r="K32" s="31"/>
-      <c r="L32" s="31"/>
-      <c r="M32" s="41"/>
-      <c r="N32" s="6">
-        <f>SUM(C32:M32)</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="O32" s="11"/>
-      <c r="P32" s="11"/>
-      <c r="Q32" s="11"/>
-      <c r="R32" s="11"/>
-      <c r="S32" s="11"/>
-      <c r="T32" s="11"/>
-      <c r="U32" s="11"/>
-      <c r="V32" s="11"/>
-      <c r="W32" s="11"/>
-      <c r="X32" s="11"/>
-      <c r="Y32" s="11"/>
-      <c r="Z32" s="11"/>
-      <c r="AA32" s="11"/>
-      <c r="AB32" s="11"/>
-      <c r="AC32" s="11"/>
-      <c r="AD32" s="11"/>
-      <c r="AE32" s="11"/>
-      <c r="AF32" s="11"/>
-    </row>
-    <row r="33" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="6">
-        <f t="shared" ref="B33:N33" si="1">SUM(B2:B32)</f>
-        <v>3.666666666666667</v>
-      </c>
-      <c r="C33" s="6">
-        <f t="shared" si="1"/>
-        <v>0.33333333333333337</v>
-      </c>
-      <c r="D33" s="6">
-        <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="E33" s="6">
-        <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="F33" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G33" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H33" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I33" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J33" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K33" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L33" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M33" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="F33" s="31">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="G33" s="31"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="31"/>
+      <c r="J33" s="31"/>
+      <c r="K33" s="31"/>
+      <c r="L33" s="31"/>
+      <c r="M33" s="41"/>
       <c r="N33" s="6">
-        <f t="shared" si="1"/>
-        <v>0.99999999999999989</v>
+        <f>SUM(C33:M33)</f>
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="O33" s="11"/>
       <c r="P33" s="11"/>
@@ -6299,55 +6282,126 @@
       <c r="AE33" s="11"/>
       <c r="AF33" s="11"/>
     </row>
-    <row r="34" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M34" s="42">
-        <f>SUM(C33:M33)</f>
-        <v>1</v>
-      </c>
+    <row r="34" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="6">
+        <f t="shared" ref="B34:N34" si="1">SUM(B2:B33)</f>
+        <v>3.666666666666667</v>
+      </c>
+      <c r="C34" s="6">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="D34" s="6">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E34" s="6">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F34" s="6">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G34" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H34" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I34" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J34" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K34" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L34" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M34" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N34" s="6">
+        <f t="shared" si="1"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="O34" s="11"/>
+      <c r="P34" s="11"/>
+      <c r="Q34" s="11"/>
+      <c r="R34" s="11"/>
+      <c r="S34" s="11"/>
+      <c r="T34" s="11"/>
+      <c r="U34" s="11"/>
+      <c r="V34" s="11"/>
+      <c r="W34" s="11"/>
+      <c r="X34" s="11"/>
+      <c r="Y34" s="11"/>
+      <c r="Z34" s="11"/>
+      <c r="AA34" s="11"/>
+      <c r="AB34" s="11"/>
+      <c r="AC34" s="11"/>
+      <c r="AD34" s="11"/>
+      <c r="AE34" s="11"/>
+      <c r="AF34" s="11"/>
     </row>
-    <row r="35" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F35" s="44" t="s">
+    <row r="35" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M35" s="42">
+        <f>SUM(C34:M34)</f>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="36" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F36" s="44" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="O36" s="11"/>
-      <c r="P36" s="11"/>
-      <c r="Q36" s="11"/>
-      <c r="R36" s="11"/>
-      <c r="S36" s="11"/>
-      <c r="T36" s="11"/>
-      <c r="U36" s="11"/>
-      <c r="V36" s="11"/>
-      <c r="W36" s="11"/>
-      <c r="X36" s="11"/>
-      <c r="Y36" s="11"/>
-      <c r="Z36" s="11"/>
-      <c r="AA36" s="11"/>
-      <c r="AB36" s="11"/>
-      <c r="AC36" s="11"/>
-      <c r="AD36" s="11"/>
-      <c r="AE36" s="11"/>
-      <c r="AF36" s="11"/>
+    <row r="37" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O37" s="11"/>
+      <c r="P37" s="11"/>
+      <c r="Q37" s="11"/>
+      <c r="R37" s="11"/>
+      <c r="S37" s="11"/>
+      <c r="T37" s="11"/>
+      <c r="U37" s="11"/>
+      <c r="V37" s="11"/>
+      <c r="W37" s="11"/>
+      <c r="X37" s="11"/>
+      <c r="Y37" s="11"/>
+      <c r="Z37" s="11"/>
+      <c r="AA37" s="11"/>
+      <c r="AB37" s="11"/>
+      <c r="AC37" s="11"/>
+      <c r="AD37" s="11"/>
+      <c r="AE37" s="11"/>
+      <c r="AF37" s="11"/>
     </row>
-    <row r="38" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="49" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="50" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="51" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="52" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="53" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="54" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="56" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7297,44 +7351,45 @@
     <row r="1002" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1003" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1004" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1005" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A14:F14"/>
-    <mergeCell ref="A22:I22"/>
-    <mergeCell ref="A31:M31"/>
+    <mergeCell ref="A23:I23"/>
+    <mergeCell ref="A32:M32"/>
   </mergeCells>
-  <conditionalFormatting sqref="C2:J3 C26:C27 I26:I27 L2:M3 E26:E27 G26:G27 L26:L27 L8:L13 I8:I13 G8:G13 E8:E13 C8:C13 L19 I19 G19 E19 C19 C4:C5 E4:E5 G4:G5 I4:I5 L4:L5 C23 C16:C17 E23 E16:E17 G23 G16:G17 I23 I16:I17 L23 L16:L17 I30 I32 L30 L32 G30 G32 E30 E32 C30 C32">
+  <conditionalFormatting sqref="C2:J3 C27:C28 I27:I28 L2:M3 E27:E28 G27:G28 L27:L28 L8:L13 I8:I13 G8:G13 E8:E13 C8:C13 L20 I20 G20 E20 C20 C4:C5 E4:E5 G4:G5 I4:I5 L4:L5 C24 C17:C18 E24 E17:E18 G24 G17:G18 I24 I17:I18 L24 L17:L18 I31 I33 L31 L33 G31 G33 E31 E33 C31 C33">
     <cfRule type="cellIs" dxfId="95" priority="178" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:M10 C25:M27 C19:M19 C2:M5 C23:M23 C16:M17 L32:M32 C30:M30 C32:J32 C12:M13 C11 E11:M11">
+  <conditionalFormatting sqref="C8:M10 C26:M28 C20:M20 C2:M5 C24:M24 C17:M18 L33:M33 C31:M31 C33:J33 C12:M13 C11 E11:M11">
     <cfRule type="cellIs" dxfId="94" priority="179" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L25 I25 G25 E25 C25">
+  <conditionalFormatting sqref="L26 I26 G26 E26 C26">
     <cfRule type="cellIs" dxfId="93" priority="180" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C25:J25 L25:M25">
+  <conditionalFormatting sqref="C26:J26 L26:M26">
     <cfRule type="cellIs" dxfId="92" priority="181" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D30 F30 H30 J30 M30">
+  <conditionalFormatting sqref="D31 F31 H31 J31 M31">
     <cfRule type="cellIs" dxfId="91" priority="182" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:M10 C25:M27 C19:M19 C2:M5 C23:M23 C16:M17 L32:M32 C30:M30 C32:J32 C12:M13 C11 E11:M11">
+  <conditionalFormatting sqref="C8:M10 C26:M28 C20:M20 C2:M5 C24:M24 C17:M18 L33:M33 C31:M31 C33:J33 C12:M13 C11 E11:M11">
     <cfRule type="cellIs" dxfId="90" priority="183" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:M10 C25:M27 C19:M19 C2:M5 C23:M23 C16:M17 L32:M32 C30:M30 C32:J32 C12:M13 C11 E11:M11">
+  <conditionalFormatting sqref="C8:M10 C26:M28 C20:M20 C2:M5 C24:M24 C17:M18 L33:M33 C31:M31 C33:J33 C12:M13 C11 E11:M11">
     <cfRule type="cellIs" dxfId="89" priority="184" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7344,82 +7399,82 @@
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K3 K9:K13 K26:K27 K17 K30">
+  <conditionalFormatting sqref="K2:K3 K9:K13 K27:K28 K18 K31">
     <cfRule type="cellIs" dxfId="87" priority="175" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K25">
+  <conditionalFormatting sqref="K26">
     <cfRule type="cellIs" dxfId="86" priority="176" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K30">
+  <conditionalFormatting sqref="K31">
     <cfRule type="cellIs" dxfId="85" priority="177" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3 N25:N27 N5 N19 N21 N8:N13 N15:N17 N23 N30 N32">
+  <conditionalFormatting sqref="N3 N26:N28 N5 N20 N22 N8:N13 N24 N31 N33 N15:N18">
     <cfRule type="cellIs" dxfId="84" priority="173" operator="equal">
       <formula>$B3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C33">
+  <conditionalFormatting sqref="C34">
     <cfRule type="cellIs" dxfId="83" priority="172" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D33:M33">
+  <conditionalFormatting sqref="D34:M34">
     <cfRule type="cellIs" dxfId="82" priority="171" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D32">
+  <conditionalFormatting sqref="D33">
     <cfRule type="cellIs" dxfId="81" priority="170" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F32">
+  <conditionalFormatting sqref="F33">
     <cfRule type="cellIs" dxfId="80" priority="169" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H32">
+  <conditionalFormatting sqref="H33">
     <cfRule type="cellIs" dxfId="79" priority="168" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J32">
+  <conditionalFormatting sqref="J33">
     <cfRule type="cellIs" dxfId="78" priority="167" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K32">
+  <conditionalFormatting sqref="K33">
     <cfRule type="cellIs" dxfId="77" priority="162" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K32">
+  <conditionalFormatting sqref="K33">
     <cfRule type="cellIs" dxfId="76" priority="163" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K32">
+  <conditionalFormatting sqref="K33">
     <cfRule type="cellIs" dxfId="75" priority="164" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K32">
+  <conditionalFormatting sqref="K33">
     <cfRule type="cellIs" dxfId="74" priority="165" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K32">
+  <conditionalFormatting sqref="K33">
     <cfRule type="cellIs" dxfId="73" priority="166" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M32">
+  <conditionalFormatting sqref="M33">
     <cfRule type="cellIs" dxfId="72" priority="161" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
@@ -7469,257 +7524,257 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
+  <conditionalFormatting sqref="K19">
     <cfRule type="cellIs" dxfId="62" priority="145" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C18 E18 G18 I18 L18">
+  <conditionalFormatting sqref="C19 E19 G19 I19 L19">
     <cfRule type="cellIs" dxfId="61" priority="148" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C18:J18 L18:M18">
+  <conditionalFormatting sqref="C19:J19 L19:M19">
     <cfRule type="cellIs" dxfId="60" priority="149" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C18:J18 L18:M18">
+  <conditionalFormatting sqref="C19:J19 L19:M19">
     <cfRule type="cellIs" dxfId="59" priority="150" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C18:J18 L18:M18">
+  <conditionalFormatting sqref="C19:J19 L19:M19">
     <cfRule type="cellIs" dxfId="58" priority="151" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
+  <conditionalFormatting sqref="K19">
     <cfRule type="cellIs" dxfId="57" priority="146" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
+  <conditionalFormatting sqref="K19">
     <cfRule type="cellIs" dxfId="56" priority="147" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L21 I21 G21 E21 C21">
+  <conditionalFormatting sqref="L22 I22 G22 E22 C22">
     <cfRule type="cellIs" dxfId="55" priority="141" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21:M21">
+  <conditionalFormatting sqref="C22:M22">
     <cfRule type="cellIs" dxfId="54" priority="142" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21:M21">
+  <conditionalFormatting sqref="C22:M22">
     <cfRule type="cellIs" dxfId="53" priority="143" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21:M21">
+  <conditionalFormatting sqref="C22:M22">
     <cfRule type="cellIs" dxfId="52" priority="144" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="K22">
+    <cfRule type="cellIs" dxfId="51" priority="140" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="K21">
-    <cfRule type="cellIs" dxfId="51" priority="140" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K20">
     <cfRule type="cellIs" dxfId="50" priority="133" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K28">
+  <conditionalFormatting sqref="K29">
     <cfRule type="cellIs" dxfId="49" priority="121" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C20 E20 G20 I20 L20">
+  <conditionalFormatting sqref="C21 E21 G21 I21 L21">
     <cfRule type="cellIs" dxfId="48" priority="136" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C20:J20 L20:M20">
+  <conditionalFormatting sqref="C21:J21 L21:M21">
     <cfRule type="cellIs" dxfId="47" priority="137" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C20:J20 L20:M20">
+  <conditionalFormatting sqref="C21:J21 L21:M21">
     <cfRule type="cellIs" dxfId="46" priority="138" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C20:J20 L20:M20">
+  <conditionalFormatting sqref="C21:J21 L21:M21">
     <cfRule type="cellIs" dxfId="45" priority="139" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K20">
+  <conditionalFormatting sqref="K21">
     <cfRule type="cellIs" dxfId="44" priority="134" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K20">
+  <conditionalFormatting sqref="K21">
     <cfRule type="cellIs" dxfId="43" priority="135" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L15 I15 G15 E15 C15">
+  <conditionalFormatting sqref="L15:L16 I15:I16 G15:G16 E15:E16 C15:C16">
     <cfRule type="cellIs" dxfId="42" priority="129" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15:M15">
+  <conditionalFormatting sqref="C15:M16">
     <cfRule type="cellIs" dxfId="41" priority="130" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15:M15">
+  <conditionalFormatting sqref="C15:M16">
     <cfRule type="cellIs" dxfId="40" priority="131" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15:M15">
+  <conditionalFormatting sqref="C15:M16">
     <cfRule type="cellIs" dxfId="39" priority="132" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K15">
+  <conditionalFormatting sqref="K15:K16">
     <cfRule type="cellIs" dxfId="38" priority="128" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28 E28 G28 I28 L28">
+  <conditionalFormatting sqref="C29 E29 G29 I29 L29">
     <cfRule type="cellIs" dxfId="37" priority="124" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28:J28 L28:M28">
+  <conditionalFormatting sqref="C29:J29 L29:M29">
     <cfRule type="cellIs" dxfId="36" priority="125" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28:J28 L28:M28">
+  <conditionalFormatting sqref="C29:J29 L29:M29">
     <cfRule type="cellIs" dxfId="35" priority="126" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28:J28 L28:M28">
+  <conditionalFormatting sqref="C29:J29 L29:M29">
     <cfRule type="cellIs" dxfId="34" priority="127" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K28">
+  <conditionalFormatting sqref="K29">
     <cfRule type="cellIs" dxfId="33" priority="122" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K28">
+  <conditionalFormatting sqref="K29">
     <cfRule type="cellIs" dxfId="32" priority="123" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24 E24 G24 I24 L24">
+  <conditionalFormatting sqref="C25 E25 G25 I25 L25">
     <cfRule type="cellIs" dxfId="31" priority="117" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24:J24 L24:M24">
+  <conditionalFormatting sqref="C25:J25 L25:M25">
     <cfRule type="cellIs" dxfId="30" priority="118" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24:J24 L24:M24">
+  <conditionalFormatting sqref="C25:J25 L25:M25">
     <cfRule type="cellIs" dxfId="29" priority="119" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24:J24 L24:M24">
+  <conditionalFormatting sqref="C25:J25 L25:M25">
     <cfRule type="cellIs" dxfId="28" priority="120" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K24">
+  <conditionalFormatting sqref="K25">
     <cfRule type="cellIs" dxfId="27" priority="114" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K24">
+  <conditionalFormatting sqref="K25">
     <cfRule type="cellIs" dxfId="26" priority="115" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K24">
+  <conditionalFormatting sqref="K25">
     <cfRule type="cellIs" dxfId="25" priority="116" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L30">
+  <conditionalFormatting sqref="L31">
     <cfRule type="cellIs" dxfId="24" priority="101" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I29 L29 G29 E29 C29">
+  <conditionalFormatting sqref="I30 L30 G30 E30 C30">
     <cfRule type="cellIs" dxfId="23" priority="109" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C29:M29">
+  <conditionalFormatting sqref="C30:M30">
     <cfRule type="cellIs" dxfId="22" priority="110" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D29 F29 H29 J29 M29">
+  <conditionalFormatting sqref="D30 F30 H30 J30 M30">
     <cfRule type="cellIs" dxfId="21" priority="111" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C29:M29">
+  <conditionalFormatting sqref="C30:M30">
     <cfRule type="cellIs" dxfId="20" priority="112" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C29:M29">
+  <conditionalFormatting sqref="C30:M30">
     <cfRule type="cellIs" dxfId="19" priority="113" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K29">
+  <conditionalFormatting sqref="K30">
     <cfRule type="cellIs" dxfId="18" priority="107" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K29">
+  <conditionalFormatting sqref="K30">
     <cfRule type="cellIs" dxfId="17" priority="108" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N29">
+  <conditionalFormatting sqref="N30">
     <cfRule type="cellIs" dxfId="16" priority="106" operator="equal">
-      <formula>$B29</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E30">
+      <formula>$B30</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31">
     <cfRule type="cellIs" dxfId="15" priority="105" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G30">
+  <conditionalFormatting sqref="G31">
     <cfRule type="cellIs" dxfId="14" priority="104" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I30">
+  <conditionalFormatting sqref="I31">
     <cfRule type="cellIs" dxfId="13" priority="103" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K30">
+  <conditionalFormatting sqref="K31">
     <cfRule type="cellIs" dxfId="12" priority="102" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
@@ -7764,22 +7819,22 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L22">
+  <conditionalFormatting sqref="L23">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J22:M22">
+  <conditionalFormatting sqref="J23:M23">
     <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J22:M22">
+  <conditionalFormatting sqref="J23:M23">
     <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J22:M22">
+  <conditionalFormatting sqref="J23:M23">
     <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
docs: documentation du jour 5
</commit_message>
<xml_diff>
--- a/docs/plannification_TPI.xlsx
+++ b/docs/plannification_TPI.xlsx
@@ -2318,7 +2318,7 @@
   <dimension ref="A1:AF1004"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5082,7 +5082,7 @@
   <dimension ref="A1:AF1005"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5755,7 +5755,9 @@
       <c r="D18" s="26"/>
       <c r="E18" s="25"/>
       <c r="F18" s="26"/>
-      <c r="G18" s="25"/>
+      <c r="G18" s="25">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="H18" s="26"/>
       <c r="I18" s="25"/>
       <c r="J18" s="26"/>
@@ -5764,7 +5766,7 @@
       <c r="M18" s="27"/>
       <c r="N18" s="6">
         <f>SUM(C18:M18)</f>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="O18" s="11"/>
       <c r="P18" s="11"/>
@@ -5831,7 +5833,9 @@
       <c r="D20" s="26"/>
       <c r="E20" s="25"/>
       <c r="F20" s="26"/>
-      <c r="G20" s="28"/>
+      <c r="G20" s="25">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="H20" s="26"/>
       <c r="I20" s="25"/>
       <c r="J20" s="26"/>
@@ -5840,7 +5844,7 @@
       <c r="M20" s="27"/>
       <c r="N20" s="6">
         <f>SUM(C20:M20)</f>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="21" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6141,7 +6145,9 @@
       <c r="D30" s="25"/>
       <c r="E30" s="25"/>
       <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
+      <c r="G30" s="25">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="H30" s="25"/>
       <c r="I30" s="25"/>
       <c r="J30" s="25"/>
@@ -6150,7 +6156,7 @@
       <c r="M30" s="29"/>
       <c r="N30" s="6">
         <f>SUM(C30:M30)</f>
-        <v>0.10416666666666667</v>
+        <v>0.125</v>
       </c>
       <c r="O30" s="11"/>
       <c r="P30" s="11"/>
@@ -6186,7 +6192,9 @@
         <v>4.8611111111111112E-2</v>
       </c>
       <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
+      <c r="G31" s="25">
+        <v>0.17361111111111113</v>
+      </c>
       <c r="H31" s="25"/>
       <c r="I31" s="25"/>
       <c r="J31" s="25"/>
@@ -6195,7 +6203,7 @@
       <c r="M31" s="40"/>
       <c r="N31" s="6">
         <f>SUM(C31:M31)</f>
-        <v>9.0277777777777776E-2</v>
+        <v>0.2638888888888889</v>
       </c>
       <c r="O31" s="11"/>
       <c r="P31" s="11"/>
@@ -6252,7 +6260,9 @@
       <c r="F33" s="31">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="G33" s="31"/>
+      <c r="G33" s="31">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="H33" s="31"/>
       <c r="I33" s="31"/>
       <c r="J33" s="31"/>
@@ -6261,7 +6271,7 @@
       <c r="M33" s="41"/>
       <c r="N33" s="6">
         <f>SUM(C33:M33)</f>
-        <v>5.5555555555555552E-2</v>
+        <v>6.9444444444444448E-2</v>
       </c>
       <c r="O33" s="11"/>
       <c r="P33" s="11"/>
@@ -6305,7 +6315,7 @@
       </c>
       <c r="G34" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="H34" s="6">
         <f t="shared" si="1"/>
@@ -6333,7 +6343,7 @@
       </c>
       <c r="N34" s="6">
         <f t="shared" si="1"/>
-        <v>1.3333333333333333</v>
+        <v>1.6666666666666665</v>
       </c>
       <c r="O34" s="11"/>
       <c r="P34" s="11"/>
@@ -6357,7 +6367,7 @@
     <row r="35" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M35" s="42">
         <f>SUM(C34:M34)</f>
-        <v>1.3333333333333333</v>
+        <v>1.6666666666666665</v>
       </c>
     </row>
     <row r="36" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
docs: documentation du jour 6
</commit_message>
<xml_diff>
--- a/docs/plannification_TPI.xlsx
+++ b/docs/plannification_TPI.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="38">
   <si>
     <t>Tâches à réaliser</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>Temps prévu</t>
+  </si>
+  <si>
+    <t>Commentaire / refactorisation</t>
   </si>
 </sst>
 </file>
@@ -5079,10 +5082,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF1005"/>
+  <dimension ref="A1:AF1006"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5528,7 +5531,9 @@
       </c>
       <c r="F12" s="26"/>
       <c r="G12" s="25"/>
-      <c r="H12" s="26"/>
+      <c r="H12" s="26">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="I12" s="25"/>
       <c r="J12" s="26"/>
       <c r="K12" s="26"/>
@@ -5536,7 +5541,7 @@
       <c r="M12" s="27"/>
       <c r="N12" s="6">
         <f t="shared" si="0"/>
-        <v>0.27083333333333331</v>
+        <v>0.35416666666666663</v>
       </c>
       <c r="O12" s="11"/>
       <c r="P12" s="11"/>
@@ -5876,7 +5881,9 @@
       <c r="E22" s="25"/>
       <c r="F22" s="26"/>
       <c r="G22" s="28"/>
-      <c r="H22" s="26"/>
+      <c r="H22" s="26">
+        <v>9.0277777777777776E-2</v>
+      </c>
       <c r="I22" s="25"/>
       <c r="J22" s="26"/>
       <c r="K22" s="26"/>
@@ -5884,83 +5891,68 @@
       <c r="M22" s="27"/>
       <c r="N22" s="6">
         <f>SUM(C22:M22)</f>
+        <v>9.0277777777777776E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="22"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="26">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="I23" s="25"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="28"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="6"/>
+    </row>
+    <row r="24" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="48"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="23"/>
+    </row>
+    <row r="25" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="17">
+        <v>0.2986111111111111</v>
+      </c>
+      <c r="C25" s="28"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="28"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="6">
+        <f>SUM(C25:M25)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="48"/>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="48"/>
-      <c r="I23" s="48"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="23"/>
-    </row>
-    <row r="24" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="17">
-        <v>0.2986111111111111</v>
-      </c>
-      <c r="C24" s="28"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="23"/>
-      <c r="N24" s="6">
-        <f>SUM(C24:M24)</f>
-        <v>0</v>
-      </c>
-      <c r="O24" s="11"/>
-      <c r="P24" s="11"/>
-      <c r="Q24" s="11"/>
-      <c r="R24" s="11"/>
-      <c r="S24" s="11"/>
-      <c r="T24" s="11"/>
-      <c r="U24" s="11"/>
-      <c r="V24" s="11"/>
-      <c r="W24" s="11"/>
-      <c r="X24" s="11"/>
-      <c r="Y24" s="11"/>
-      <c r="Z24" s="11"/>
-      <c r="AA24" s="11"/>
-      <c r="AB24" s="11"/>
-      <c r="AC24" s="11"/>
-      <c r="AD24" s="11"/>
-      <c r="AE24" s="11"/>
-      <c r="AF24" s="11"/>
-    </row>
-    <row r="25" spans="1:32" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="5"/>
       <c r="O25" s="11"/>
       <c r="P25" s="11"/>
       <c r="Q25" s="11"/>
@@ -5980,26 +5972,22 @@
       <c r="AE25" s="11"/>
       <c r="AF25" s="11"/>
     </row>
-    <row r="26" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="26"/>
-      <c r="L26" s="25"/>
-      <c r="M26" s="27"/>
-      <c r="N26" s="6">
-        <f>SUM(C26:M26)</f>
-        <v>0</v>
-      </c>
+    <row r="26" spans="1:32" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="5"/>
       <c r="O26" s="11"/>
       <c r="P26" s="11"/>
       <c r="Q26" s="11"/>
@@ -6021,7 +6009,7 @@
     </row>
     <row r="27" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="35" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B27" s="24"/>
       <c r="C27" s="25"/>
@@ -6060,14 +6048,14 @@
     </row>
     <row r="28" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="35" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B28" s="24"/>
-      <c r="C28" s="28"/>
+      <c r="C28" s="25"/>
       <c r="D28" s="26"/>
-      <c r="E28" s="28"/>
+      <c r="E28" s="25"/>
       <c r="F28" s="26"/>
-      <c r="G28" s="28"/>
+      <c r="G28" s="25"/>
       <c r="H28" s="26"/>
       <c r="I28" s="25"/>
       <c r="J28" s="26"/>
@@ -6097,22 +6085,26 @@
       <c r="AE28" s="11"/>
       <c r="AF28" s="11"/>
     </row>
-    <row r="29" spans="1:32" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="5"/>
+    <row r="29" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="24"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="26"/>
+      <c r="K29" s="26"/>
+      <c r="L29" s="25"/>
+      <c r="M29" s="27"/>
+      <c r="N29" s="6">
+        <f>SUM(C29:M29)</f>
+        <v>0</v>
+      </c>
       <c r="O29" s="11"/>
       <c r="P29" s="11"/>
       <c r="Q29" s="11"/>
@@ -6132,32 +6124,22 @@
       <c r="AE29" s="11"/>
       <c r="AF29" s="11"/>
     </row>
-    <row r="30" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="C30" s="25">
-        <v>0.10416666666666667</v>
-      </c>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="H30" s="25"/>
-      <c r="I30" s="25"/>
-      <c r="J30" s="25"/>
-      <c r="K30" s="25"/>
-      <c r="L30" s="25"/>
-      <c r="M30" s="29"/>
-      <c r="N30" s="6">
-        <f>SUM(C30:M30)</f>
-        <v>0.125</v>
-      </c>
+    <row r="30" spans="1:32" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="5"/>
       <c r="O30" s="11"/>
       <c r="P30" s="11"/>
       <c r="Q30" s="11"/>
@@ -6178,32 +6160,32 @@
       <c r="AF30" s="11"/>
     </row>
     <row r="31" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="32" t="s">
-        <v>4</v>
+      <c r="A31" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="B31" s="24">
-        <v>1.0416666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="C31" s="25">
-        <v>4.1666666666666664E-2</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="D31" s="25"/>
-      <c r="E31" s="25">
-        <v>4.8611111111111112E-2</v>
-      </c>
+      <c r="E31" s="25"/>
       <c r="F31" s="25"/>
       <c r="G31" s="25">
-        <v>0.17361111111111113</v>
-      </c>
-      <c r="H31" s="25"/>
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="H31" s="25">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="I31" s="25"/>
       <c r="J31" s="25"/>
       <c r="K31" s="25"/>
-      <c r="L31" s="39"/>
-      <c r="M31" s="40"/>
+      <c r="L31" s="25"/>
+      <c r="M31" s="29"/>
       <c r="N31" s="6">
         <f>SUM(C31:M31)</f>
-        <v>0.2638888888888889</v>
+        <v>0.14583333333333334</v>
       </c>
       <c r="O31" s="11"/>
       <c r="P31" s="11"/>
@@ -6224,126 +6206,105 @@
       <c r="AE31" s="11"/>
       <c r="AF31" s="11"/>
     </row>
-    <row r="32" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="47" t="s">
+    <row r="32" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="24">
+        <v>1.0416666666666667</v>
+      </c>
+      <c r="C32" s="25">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25">
+        <v>4.8611111111111112E-2</v>
+      </c>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25">
+        <v>0.17361111111111113</v>
+      </c>
+      <c r="H32" s="25">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="I32" s="25"/>
+      <c r="J32" s="25"/>
+      <c r="K32" s="25"/>
+      <c r="L32" s="39"/>
+      <c r="M32" s="40"/>
+      <c r="N32" s="6">
+        <f>SUM(C32:M32)</f>
+        <v>0.34722222222222221</v>
+      </c>
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="11"/>
+      <c r="S32" s="11"/>
+      <c r="T32" s="11"/>
+      <c r="U32" s="11"/>
+      <c r="V32" s="11"/>
+      <c r="W32" s="11"/>
+      <c r="X32" s="11"/>
+      <c r="Y32" s="11"/>
+      <c r="Z32" s="11"/>
+      <c r="AA32" s="11"/>
+      <c r="AB32" s="11"/>
+      <c r="AC32" s="11"/>
+      <c r="AD32" s="11"/>
+      <c r="AE32" s="11"/>
+      <c r="AF32" s="11"/>
+    </row>
+    <row r="33" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="48"/>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="48"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="48"/>
-      <c r="H32" s="48"/>
-      <c r="I32" s="48"/>
-      <c r="J32" s="48"/>
-      <c r="K32" s="48"/>
-      <c r="L32" s="48"/>
-      <c r="M32" s="49"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="48"/>
+      <c r="D33" s="48"/>
+      <c r="E33" s="48"/>
+      <c r="F33" s="48"/>
+      <c r="G33" s="48"/>
+      <c r="H33" s="48"/>
+      <c r="I33" s="48"/>
+      <c r="J33" s="48"/>
+      <c r="K33" s="48"/>
+      <c r="L33" s="48"/>
+      <c r="M33" s="49"/>
     </row>
-    <row r="33" spans="1:32" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="33" t="s">
+    <row r="34" spans="1:32" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="B33" s="30">
+      <c r="B34" s="30">
         <v>0.15277777777777776</v>
       </c>
-      <c r="C33" s="31">
+      <c r="C34" s="31">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="D33" s="31">
+      <c r="D34" s="31">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="E33" s="31">
+      <c r="E34" s="31">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="F33" s="31">
+      <c r="F34" s="31">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="G33" s="31">
+      <c r="G34" s="31">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="H33" s="31"/>
-      <c r="I33" s="31"/>
-      <c r="J33" s="31"/>
-      <c r="K33" s="31"/>
-      <c r="L33" s="31"/>
-      <c r="M33" s="41"/>
-      <c r="N33" s="6">
-        <f>SUM(C33:M33)</f>
-        <v>6.9444444444444448E-2</v>
-      </c>
-      <c r="O33" s="11"/>
-      <c r="P33" s="11"/>
-      <c r="Q33" s="11"/>
-      <c r="R33" s="11"/>
-      <c r="S33" s="11"/>
-      <c r="T33" s="11"/>
-      <c r="U33" s="11"/>
-      <c r="V33" s="11"/>
-      <c r="W33" s="11"/>
-      <c r="X33" s="11"/>
-      <c r="Y33" s="11"/>
-      <c r="Z33" s="11"/>
-      <c r="AA33" s="11"/>
-      <c r="AB33" s="11"/>
-      <c r="AC33" s="11"/>
-      <c r="AD33" s="11"/>
-      <c r="AE33" s="11"/>
-      <c r="AF33" s="11"/>
-    </row>
-    <row r="34" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="6">
-        <f t="shared" ref="B34:N34" si="1">SUM(B2:B33)</f>
-        <v>3.666666666666667</v>
-      </c>
-      <c r="C34" s="6">
-        <f t="shared" si="1"/>
-        <v>0.33333333333333337</v>
-      </c>
-      <c r="D34" s="6">
-        <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="E34" s="6">
-        <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="F34" s="6">
-        <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="G34" s="6">
-        <f t="shared" si="1"/>
-        <v>0.33333333333333337</v>
-      </c>
-      <c r="H34" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I34" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J34" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K34" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L34" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M34" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="H34" s="31">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="I34" s="31"/>
+      <c r="J34" s="31"/>
+      <c r="K34" s="31"/>
+      <c r="L34" s="31"/>
+      <c r="M34" s="41"/>
       <c r="N34" s="6">
-        <f t="shared" si="1"/>
-        <v>1.6666666666666665</v>
+        <f>SUM(C34:M34)</f>
+        <v>8.3333333333333343E-2</v>
       </c>
       <c r="O34" s="11"/>
       <c r="P34" s="11"/>
@@ -6365,37 +6326,108 @@
       <c r="AF34" s="11"/>
     </row>
     <row r="35" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M35" s="42">
-        <f>SUM(C34:M34)</f>
-        <v>1.6666666666666665</v>
-      </c>
+      <c r="B35" s="6">
+        <f t="shared" ref="B35:N35" si="1">SUM(B2:B34)</f>
+        <v>3.666666666666667</v>
+      </c>
+      <c r="C35" s="6">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="D35" s="6">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E35" s="6">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F35" s="6">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G35" s="6">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="H35" s="6">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I35" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J35" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K35" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L35" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M35" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N35" s="6">
+        <f t="shared" si="1"/>
+        <v>1.9583333333333333</v>
+      </c>
+      <c r="O35" s="11"/>
+      <c r="P35" s="11"/>
+      <c r="Q35" s="11"/>
+      <c r="R35" s="11"/>
+      <c r="S35" s="11"/>
+      <c r="T35" s="11"/>
+      <c r="U35" s="11"/>
+      <c r="V35" s="11"/>
+      <c r="W35" s="11"/>
+      <c r="X35" s="11"/>
+      <c r="Y35" s="11"/>
+      <c r="Z35" s="11"/>
+      <c r="AA35" s="11"/>
+      <c r="AB35" s="11"/>
+      <c r="AC35" s="11"/>
+      <c r="AD35" s="11"/>
+      <c r="AE35" s="11"/>
+      <c r="AF35" s="11"/>
     </row>
     <row r="36" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F36" s="44" t="s">
-        <v>28</v>
+      <c r="M36" s="42">
+        <f>SUM(C35:M35)</f>
+        <v>1.9999999999999998</v>
       </c>
     </row>
     <row r="37" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="O37" s="11"/>
-      <c r="P37" s="11"/>
-      <c r="Q37" s="11"/>
-      <c r="R37" s="11"/>
-      <c r="S37" s="11"/>
-      <c r="T37" s="11"/>
-      <c r="U37" s="11"/>
-      <c r="V37" s="11"/>
-      <c r="W37" s="11"/>
-      <c r="X37" s="11"/>
-      <c r="Y37" s="11"/>
-      <c r="Z37" s="11"/>
-      <c r="AA37" s="11"/>
-      <c r="AB37" s="11"/>
-      <c r="AC37" s="11"/>
-      <c r="AD37" s="11"/>
-      <c r="AE37" s="11"/>
-      <c r="AF37" s="11"/>
+      <c r="F37" s="44" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="39" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O38" s="11"/>
+      <c r="P38" s="11"/>
+      <c r="Q38" s="11"/>
+      <c r="R38" s="11"/>
+      <c r="S38" s="11"/>
+      <c r="T38" s="11"/>
+      <c r="U38" s="11"/>
+      <c r="V38" s="11"/>
+      <c r="W38" s="11"/>
+      <c r="X38" s="11"/>
+      <c r="Y38" s="11"/>
+      <c r="Z38" s="11"/>
+      <c r="AA38" s="11"/>
+      <c r="AB38" s="11"/>
+      <c r="AC38" s="11"/>
+      <c r="AD38" s="11"/>
+      <c r="AE38" s="11"/>
+      <c r="AF38" s="11"/>
+    </row>
     <row r="40" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="41" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="42" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6412,7 +6444,7 @@
     <row r="53" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="54" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="55" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="59" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7362,44 +7394,45 @@
     <row r="1003" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1004" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1005" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1006" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A14:F14"/>
-    <mergeCell ref="A23:I23"/>
-    <mergeCell ref="A32:M32"/>
+    <mergeCell ref="A24:I24"/>
+    <mergeCell ref="A33:M33"/>
   </mergeCells>
-  <conditionalFormatting sqref="C2:J3 C27:C28 I27:I28 L2:M3 E27:E28 G27:G28 L27:L28 L8:L13 I8:I13 G8:G13 E8:E13 C8:C13 L20 I20 G20 E20 C20 C4:C5 E4:E5 G4:G5 I4:I5 L4:L5 C24 C17:C18 E24 E17:E18 G24 G17:G18 I24 I17:I18 L24 L17:L18 I31 I33 L31 L33 G31 G33 E31 E33 C31 C33">
+  <conditionalFormatting sqref="C2:J3 C28:C29 I28:I29 L2:M3 E28:E29 G28:G29 L28:L29 L8:L13 I8:I13 G8:G13 E8:E13 C8:C13 L20 I20 G20 E20 C20 C4:C5 E4:E5 G4:G5 I4:I5 L4:L5 C25 C17:C18 E25 E17:E18 G25 G17:G18 I25 I17:I18 L25 L17:L18 I32 I34 L32 L34 G32 G34 E32 E34 C32 C34">
     <cfRule type="cellIs" dxfId="95" priority="178" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:M10 C26:M28 C20:M20 C2:M5 C24:M24 C17:M18 L33:M33 C31:M31 C33:J33 C12:M13 C11 E11:M11">
+  <conditionalFormatting sqref="C8:M10 C27:M29 C20:M20 C2:M5 C25:M25 C17:M18 L34:M34 C32:M32 C34:J34 C12:M13 C11 E11:M11">
     <cfRule type="cellIs" dxfId="94" priority="179" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L26 I26 G26 E26 C26">
+  <conditionalFormatting sqref="L27 I27 G27 E27 C27">
     <cfRule type="cellIs" dxfId="93" priority="180" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C26:J26 L26:M26">
+  <conditionalFormatting sqref="C27:J27 L27:M27">
     <cfRule type="cellIs" dxfId="92" priority="181" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D31 F31 H31 J31 M31">
+  <conditionalFormatting sqref="D32 F32 H32 J32 M32">
     <cfRule type="cellIs" dxfId="91" priority="182" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:M10 C26:M28 C20:M20 C2:M5 C24:M24 C17:M18 L33:M33 C31:M31 C33:J33 C12:M13 C11 E11:M11">
+  <conditionalFormatting sqref="C8:M10 C27:M29 C20:M20 C2:M5 C25:M25 C17:M18 L34:M34 C32:M32 C34:J34 C12:M13 C11 E11:M11">
     <cfRule type="cellIs" dxfId="90" priority="183" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:M10 C26:M28 C20:M20 C2:M5 C24:M24 C17:M18 L33:M33 C31:M31 C33:J33 C12:M13 C11 E11:M11">
+  <conditionalFormatting sqref="C8:M10 C27:M29 C20:M20 C2:M5 C25:M25 C17:M18 L34:M34 C32:M32 C34:J34 C12:M13 C11 E11:M11">
     <cfRule type="cellIs" dxfId="89" priority="184" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7409,82 +7442,82 @@
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K3 K9:K13 K27:K28 K18 K31">
+  <conditionalFormatting sqref="K2:K3 K9:K13 K28:K29 K18 K32">
     <cfRule type="cellIs" dxfId="87" priority="175" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K26">
+  <conditionalFormatting sqref="K27">
     <cfRule type="cellIs" dxfId="86" priority="176" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K31">
+  <conditionalFormatting sqref="K32">
     <cfRule type="cellIs" dxfId="85" priority="177" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3 N26:N28 N5 N20 N22 N8:N13 N24 N31 N33 N15:N18">
+  <conditionalFormatting sqref="N3 N27:N29 N5 N20 N22:N23 N8:N13 N25 N32 N34 N15:N18">
     <cfRule type="cellIs" dxfId="84" priority="173" operator="equal">
       <formula>$B3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
+  <conditionalFormatting sqref="C35">
     <cfRule type="cellIs" dxfId="83" priority="172" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34:M34">
+  <conditionalFormatting sqref="D35:M35">
     <cfRule type="cellIs" dxfId="82" priority="171" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D33">
+  <conditionalFormatting sqref="D34">
     <cfRule type="cellIs" dxfId="81" priority="170" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F33">
+  <conditionalFormatting sqref="F34">
     <cfRule type="cellIs" dxfId="80" priority="169" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H33">
+  <conditionalFormatting sqref="H34">
     <cfRule type="cellIs" dxfId="79" priority="168" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J33">
+  <conditionalFormatting sqref="J34">
     <cfRule type="cellIs" dxfId="78" priority="167" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K33">
+  <conditionalFormatting sqref="K34">
     <cfRule type="cellIs" dxfId="77" priority="162" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K33">
+  <conditionalFormatting sqref="K34">
     <cfRule type="cellIs" dxfId="76" priority="163" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K33">
+  <conditionalFormatting sqref="K34">
     <cfRule type="cellIs" dxfId="75" priority="164" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K33">
+  <conditionalFormatting sqref="K34">
     <cfRule type="cellIs" dxfId="74" priority="165" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K33">
+  <conditionalFormatting sqref="K34">
     <cfRule type="cellIs" dxfId="73" priority="166" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M33">
+  <conditionalFormatting sqref="M34">
     <cfRule type="cellIs" dxfId="72" priority="161" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
@@ -7569,27 +7602,27 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L22 I22 G22 E22 C22">
+  <conditionalFormatting sqref="L22:L23 I22:I23 G22:G23 E22:E23 C22:C23">
     <cfRule type="cellIs" dxfId="55" priority="141" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C22:M22">
+  <conditionalFormatting sqref="C22:M23">
     <cfRule type="cellIs" dxfId="54" priority="142" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C22:M22">
+  <conditionalFormatting sqref="C22:M23">
     <cfRule type="cellIs" dxfId="53" priority="143" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C22:M22">
+  <conditionalFormatting sqref="C22:M23">
     <cfRule type="cellIs" dxfId="52" priority="144" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K22">
+  <conditionalFormatting sqref="K22:K23">
     <cfRule type="cellIs" dxfId="51" priority="140" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7599,7 +7632,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K29">
+  <conditionalFormatting sqref="K30">
     <cfRule type="cellIs" dxfId="49" priority="121" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7659,132 +7692,132 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C29 E29 G29 I29 L29">
+  <conditionalFormatting sqref="C30 E30 G30 I30 L30">
     <cfRule type="cellIs" dxfId="37" priority="124" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C29:J29 L29:M29">
+  <conditionalFormatting sqref="C30:J30 L30:M30">
     <cfRule type="cellIs" dxfId="36" priority="125" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C29:J29 L29:M29">
+  <conditionalFormatting sqref="C30:J30 L30:M30">
     <cfRule type="cellIs" dxfId="35" priority="126" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C29:J29 L29:M29">
+  <conditionalFormatting sqref="C30:J30 L30:M30">
     <cfRule type="cellIs" dxfId="34" priority="127" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K29">
+  <conditionalFormatting sqref="K30">
     <cfRule type="cellIs" dxfId="33" priority="122" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K29">
+  <conditionalFormatting sqref="K30">
     <cfRule type="cellIs" dxfId="32" priority="123" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C25 E25 G25 I25 L25">
+  <conditionalFormatting sqref="C26 E26 G26 I26 L26">
     <cfRule type="cellIs" dxfId="31" priority="117" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C25:J25 L25:M25">
+  <conditionalFormatting sqref="C26:J26 L26:M26">
     <cfRule type="cellIs" dxfId="30" priority="118" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C25:J25 L25:M25">
+  <conditionalFormatting sqref="C26:J26 L26:M26">
     <cfRule type="cellIs" dxfId="29" priority="119" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C25:J25 L25:M25">
+  <conditionalFormatting sqref="C26:J26 L26:M26">
     <cfRule type="cellIs" dxfId="28" priority="120" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K25">
+  <conditionalFormatting sqref="K26">
     <cfRule type="cellIs" dxfId="27" priority="114" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K25">
+  <conditionalFormatting sqref="K26">
     <cfRule type="cellIs" dxfId="26" priority="115" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K25">
+  <conditionalFormatting sqref="K26">
     <cfRule type="cellIs" dxfId="25" priority="116" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L31">
+  <conditionalFormatting sqref="L32">
     <cfRule type="cellIs" dxfId="24" priority="101" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I30 L30 G30 E30 C30">
+  <conditionalFormatting sqref="I31 L31 G31 E31 C31">
     <cfRule type="cellIs" dxfId="23" priority="109" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C30:M30">
+  <conditionalFormatting sqref="C31:M31">
     <cfRule type="cellIs" dxfId="22" priority="110" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D30 F30 H30 J30 M30">
+  <conditionalFormatting sqref="D31 F31 H31 J31 M31">
     <cfRule type="cellIs" dxfId="21" priority="111" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C30:M30">
+  <conditionalFormatting sqref="C31:M31">
     <cfRule type="cellIs" dxfId="20" priority="112" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C30:M30">
+  <conditionalFormatting sqref="C31:M31">
     <cfRule type="cellIs" dxfId="19" priority="113" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K30">
+  <conditionalFormatting sqref="K31">
     <cfRule type="cellIs" dxfId="18" priority="107" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K30">
+  <conditionalFormatting sqref="K31">
     <cfRule type="cellIs" dxfId="17" priority="108" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N30">
+  <conditionalFormatting sqref="N31">
     <cfRule type="cellIs" dxfId="16" priority="106" operator="equal">
-      <formula>$B30</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
+      <formula>$B31</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E32">
     <cfRule type="cellIs" dxfId="15" priority="105" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G31">
+  <conditionalFormatting sqref="G32">
     <cfRule type="cellIs" dxfId="14" priority="104" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I31">
+  <conditionalFormatting sqref="I32">
     <cfRule type="cellIs" dxfId="13" priority="103" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K31">
+  <conditionalFormatting sqref="K32">
     <cfRule type="cellIs" dxfId="12" priority="102" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
@@ -7829,22 +7862,22 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L23">
+  <conditionalFormatting sqref="L24">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J23:M23">
+  <conditionalFormatting sqref="J24:M24">
     <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J23:M23">
+  <conditionalFormatting sqref="J24:M24">
     <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J23:M23">
+  <conditionalFormatting sqref="J24:M24">
     <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
docs: documentation du jour 7
</commit_message>
<xml_diff>
--- a/docs/plannification_TPI.xlsx
+++ b/docs/plannification_TPI.xlsx
@@ -578,7 +578,27 @@
     <cellStyle name="Insatisfaisant" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="188">
+  <dxfs count="189">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1238,16 +1258,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFB8CCE4"/>
           <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2321,7 +2331,7 @@
   <dimension ref="A1:AF1004"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4616,462 +4626,462 @@
     <mergeCell ref="A14:F14"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:J3 C26:C27 I26:I27 L2:M3 E26:E27 G26:G27 L26:L27 L8:L13 I8:I13 G8:G13 E8:E13 C8:C13 L19 I19 G19 E19 C19 C4:C5 E4:E6 G4:G6 I4:I6 L4:L6 C23 C16:C17 E23 E16:E17 G23 G16:G17 I23 I16:I17 L23 L16:L17 I30 I32 L30 L32 G30 G32 E30 E32 C30 C32">
-    <cfRule type="cellIs" dxfId="187" priority="194" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="188" priority="194" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:M13 C25:M27 C19:M19 C2:M5 C23:M23 C16:M17 D6:M6 L32:M32 C30:M30 C32:J32">
-    <cfRule type="cellIs" dxfId="186" priority="195" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="187" priority="195" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L25 I25 G25 E25 C25">
-    <cfRule type="cellIs" dxfId="185" priority="196" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="186" priority="196" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:J25 L25:M25">
-    <cfRule type="cellIs" dxfId="184" priority="197" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="185" priority="197" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30 F30 H30 J30 M30">
-    <cfRule type="cellIs" dxfId="183" priority="198" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="184" priority="198" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:M13 C25:M27 C19:M19 C2:M5 C23:M23 C16:M17 D6:M6 L32:M32 C30:M30 C32:J32">
-    <cfRule type="cellIs" dxfId="182" priority="201" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="183" priority="201" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:M13 C25:M27 C19:M19 C2:M5 C23:M23 C16:M17 D6:M6 L32:M32 C30:M30 C32:J32">
-    <cfRule type="cellIs" dxfId="181" priority="202" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="182" priority="202" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K3">
-    <cfRule type="cellIs" dxfId="180" priority="186" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="181" priority="186" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K3 K9:K13 K26:K27 K17 K30">
-    <cfRule type="cellIs" dxfId="179" priority="187" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="180" priority="187" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K25">
-    <cfRule type="cellIs" dxfId="178" priority="188" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="179" priority="188" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="cellIs" dxfId="177" priority="189" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="178" priority="189" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3 N25:N27 N5 N19 N21 N8:N13 N15:N17 N23 N30 N32">
-    <cfRule type="cellIs" dxfId="176" priority="184" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="184" operator="equal">
       <formula>$B3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="cellIs" dxfId="175" priority="181" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="181" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33:M33">
-    <cfRule type="cellIs" dxfId="174" priority="180" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="180" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32">
-    <cfRule type="cellIs" dxfId="173" priority="177" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="174" priority="177" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F32">
-    <cfRule type="cellIs" dxfId="172" priority="176" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="173" priority="176" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="cellIs" dxfId="171" priority="175" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="172" priority="175" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J32">
-    <cfRule type="cellIs" dxfId="170" priority="174" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="171" priority="174" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="169" priority="169" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="170" priority="169" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="168" priority="170" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="169" priority="170" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="167" priority="171" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="168" priority="171" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="166" priority="172" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="167" priority="172" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="165" priority="173" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="166" priority="173" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M32">
-    <cfRule type="cellIs" dxfId="164" priority="168" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="165" priority="168" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2">
-    <cfRule type="cellIs" dxfId="163" priority="167" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="167" operator="equal">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4">
-    <cfRule type="cellIs" dxfId="162" priority="166" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="166" operator="equal">
       <formula>$B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7 E7 G7 I7 L7">
-    <cfRule type="cellIs" dxfId="161" priority="162" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="162" priority="162" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:J7 L7:M7">
-    <cfRule type="cellIs" dxfId="160" priority="163" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="161" priority="163" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:J7 L7:M7">
-    <cfRule type="cellIs" dxfId="159" priority="164" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="160" priority="164" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:J7 L7:M7">
-    <cfRule type="cellIs" dxfId="158" priority="165" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="159" priority="165" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="157" priority="159" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="158" priority="159" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="156" priority="160" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="157" priority="160" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="155" priority="161" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="156" priority="161" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="154" priority="152" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="155" priority="152" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18 E18 G18 I18 L18">
-    <cfRule type="cellIs" dxfId="153" priority="155" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="154" priority="155" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:J18 L18:M18">
-    <cfRule type="cellIs" dxfId="152" priority="156" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="153" priority="156" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:J18 L18:M18">
-    <cfRule type="cellIs" dxfId="151" priority="157" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="152" priority="157" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:J18 L18:M18">
-    <cfRule type="cellIs" dxfId="150" priority="158" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="151" priority="158" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="149" priority="153" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="150" priority="153" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="148" priority="154" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="149" priority="154" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L21 I21 G21 E21 C21">
-    <cfRule type="cellIs" dxfId="147" priority="143" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="148" priority="143" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:M21">
-    <cfRule type="cellIs" dxfId="146" priority="144" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="147" priority="144" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:M21">
-    <cfRule type="cellIs" dxfId="145" priority="145" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="146" priority="145" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:M21">
-    <cfRule type="cellIs" dxfId="144" priority="146" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="145" priority="146" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21">
-    <cfRule type="cellIs" dxfId="143" priority="142" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="144" priority="142" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="cellIs" dxfId="142" priority="134" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="143" priority="134" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28">
-    <cfRule type="cellIs" dxfId="141" priority="121" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="142" priority="121" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20 E20 G20 I20 L20">
-    <cfRule type="cellIs" dxfId="140" priority="137" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="141" priority="137" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:J20 L20:M20">
-    <cfRule type="cellIs" dxfId="139" priority="138" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="140" priority="138" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:J20 L20:M20">
-    <cfRule type="cellIs" dxfId="138" priority="139" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="139" priority="139" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:J20 L20:M20">
-    <cfRule type="cellIs" dxfId="137" priority="140" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="138" priority="140" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="cellIs" dxfId="136" priority="135" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="137" priority="135" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="cellIs" dxfId="135" priority="136" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="136" priority="136" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L15 I15 G15 E15 C15">
-    <cfRule type="cellIs" dxfId="134" priority="130" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="135" priority="130" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:M15">
-    <cfRule type="cellIs" dxfId="133" priority="131" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="134" priority="131" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:M15">
-    <cfRule type="cellIs" dxfId="132" priority="132" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="133" priority="132" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:M15">
-    <cfRule type="cellIs" dxfId="131" priority="133" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="132" priority="133" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="cellIs" dxfId="130" priority="129" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="131" priority="129" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28 E28 G28 I28 L28">
-    <cfRule type="cellIs" dxfId="129" priority="124" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="130" priority="124" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:J28 L28:M28">
-    <cfRule type="cellIs" dxfId="128" priority="125" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="129" priority="125" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:J28 L28:M28">
-    <cfRule type="cellIs" dxfId="127" priority="126" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="128" priority="126" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:J28 L28:M28">
-    <cfRule type="cellIs" dxfId="126" priority="127" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="127" priority="127" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28">
-    <cfRule type="cellIs" dxfId="125" priority="122" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="126" priority="122" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28">
-    <cfRule type="cellIs" dxfId="124" priority="123" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="125" priority="123" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24 E24 G24 I24 L24">
-    <cfRule type="cellIs" dxfId="123" priority="117" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="124" priority="117" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:J24 L24:M24">
-    <cfRule type="cellIs" dxfId="122" priority="118" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="123" priority="118" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:J24 L24:M24">
-    <cfRule type="cellIs" dxfId="121" priority="119" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="122" priority="119" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:J24 L24:M24">
-    <cfRule type="cellIs" dxfId="120" priority="120" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="121" priority="120" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="119" priority="114" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="120" priority="114" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="118" priority="115" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="119" priority="115" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="117" priority="116" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="118" priority="116" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L30">
-    <cfRule type="cellIs" dxfId="116" priority="101" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="117" priority="101" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I29 L29 G29 E29 C29">
-    <cfRule type="cellIs" dxfId="115" priority="109" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="116" priority="109" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29:M29">
-    <cfRule type="cellIs" dxfId="114" priority="110" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="115" priority="110" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29 F29 H29 J29 M29">
-    <cfRule type="cellIs" dxfId="113" priority="111" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="114" priority="111" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29:M29">
-    <cfRule type="cellIs" dxfId="112" priority="112" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="113" priority="112" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29:M29">
-    <cfRule type="cellIs" dxfId="111" priority="113" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="112" priority="113" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K29">
-    <cfRule type="cellIs" dxfId="110" priority="107" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="111" priority="107" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K29">
-    <cfRule type="cellIs" dxfId="109" priority="108" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="110" priority="108" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N29">
-    <cfRule type="cellIs" dxfId="108" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="106" operator="equal">
       <formula>$B29</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="cellIs" dxfId="107" priority="105" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="108" priority="105" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30">
-    <cfRule type="cellIs" dxfId="106" priority="104" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="107" priority="104" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30">
-    <cfRule type="cellIs" dxfId="105" priority="103" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="106" priority="103" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="cellIs" dxfId="104" priority="102" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="105" priority="102" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14 I14 L14">
-    <cfRule type="cellIs" dxfId="103" priority="81" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="104" priority="81" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14:M14">
-    <cfRule type="cellIs" dxfId="102" priority="82" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="103" priority="82" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14:M14">
-    <cfRule type="cellIs" dxfId="101" priority="83" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="102" priority="83" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14:M14">
-    <cfRule type="cellIs" dxfId="100" priority="84" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="101" priority="84" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L22">
-    <cfRule type="cellIs" dxfId="99" priority="57" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="100" priority="57" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:M22">
-    <cfRule type="cellIs" dxfId="98" priority="58" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="99" priority="58" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:M22">
-    <cfRule type="cellIs" dxfId="97" priority="59" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="98" priority="59" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:M22">
-    <cfRule type="cellIs" dxfId="96" priority="60" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="97" priority="60" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5085,7 +5095,7 @@
   <dimension ref="A1:AF1006"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="P37" sqref="P37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5531,17 +5541,13 @@
       </c>
       <c r="F12" s="26"/>
       <c r="G12" s="25"/>
-      <c r="H12" s="26">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="I12" s="25"/>
       <c r="J12" s="26"/>
       <c r="K12" s="26"/>
       <c r="L12" s="25"/>
       <c r="M12" s="27"/>
       <c r="N12" s="6">
         <f t="shared" si="0"/>
-        <v>0.35416666666666663</v>
+        <v>0.27083333333333331</v>
       </c>
       <c r="O12" s="11"/>
       <c r="P12" s="11"/>
@@ -5898,7 +5904,7 @@
       <c r="A23" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="22"/>
+      <c r="B23" s="24"/>
       <c r="C23" s="28"/>
       <c r="D23" s="26"/>
       <c r="E23" s="25"/>
@@ -5912,7 +5918,10 @@
       <c r="K23" s="26"/>
       <c r="L23" s="28"/>
       <c r="M23" s="23"/>
-      <c r="N23" s="6"/>
+      <c r="N23" s="6">
+        <f>SUM(C23:M23)</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
     </row>
     <row r="24" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="47" t="s">
@@ -5943,15 +5952,19 @@
       <c r="E25" s="25"/>
       <c r="F25" s="26"/>
       <c r="G25" s="28"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="25"/>
+      <c r="H25" s="26">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="I25" s="25">
+        <v>0.125</v>
+      </c>
       <c r="J25" s="26"/>
       <c r="K25" s="26"/>
       <c r="L25" s="28"/>
       <c r="M25" s="23"/>
       <c r="N25" s="6">
         <f>SUM(C25:M25)</f>
-        <v>0</v>
+        <v>0.20833333333333331</v>
       </c>
       <c r="O25" s="11"/>
       <c r="P25" s="11"/>
@@ -6227,14 +6240,16 @@
       <c r="H32" s="25">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="I32" s="25"/>
+      <c r="I32" s="25">
+        <v>0.19444444444444445</v>
+      </c>
       <c r="J32" s="25"/>
       <c r="K32" s="25"/>
       <c r="L32" s="39"/>
       <c r="M32" s="40"/>
       <c r="N32" s="6">
         <f>SUM(C32:M32)</f>
-        <v>0.34722222222222221</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="O32" s="11"/>
       <c r="P32" s="11"/>
@@ -6297,14 +6312,16 @@
       <c r="H34" s="31">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="I34" s="31"/>
+      <c r="I34" s="31">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="J34" s="31"/>
       <c r="K34" s="31"/>
       <c r="L34" s="31"/>
       <c r="M34" s="41"/>
       <c r="N34" s="6">
         <f>SUM(C34:M34)</f>
-        <v>8.3333333333333343E-2</v>
+        <v>9.7222222222222238E-2</v>
       </c>
       <c r="O34" s="11"/>
       <c r="P34" s="11"/>
@@ -6352,11 +6369,11 @@
       </c>
       <c r="H35" s="6">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="I35" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="J35" s="6">
         <f t="shared" si="1"/>
@@ -6376,7 +6393,7 @@
       </c>
       <c r="N35" s="6">
         <f t="shared" si="1"/>
-        <v>1.9583333333333333</v>
+        <v>2.333333333333333</v>
       </c>
       <c r="O35" s="11"/>
       <c r="P35" s="11"/>
@@ -6400,7 +6417,7 @@
     <row r="36" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M36" s="42">
         <f>SUM(C35:M35)</f>
-        <v>1.9999999999999998</v>
+        <v>2.3333333333333335</v>
       </c>
     </row>
     <row r="37" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -7402,483 +7419,483 @@
     <mergeCell ref="A24:I24"/>
     <mergeCell ref="A33:M33"/>
   </mergeCells>
-  <conditionalFormatting sqref="C2:J3 C28:C29 I28:I29 L2:M3 E28:E29 G28:G29 L28:L29 L8:L13 I8:I13 G8:G13 E8:E13 C8:C13 L20 I20 G20 E20 C20 C4:C5 E4:E5 G4:G5 I4:I5 L4:L5 C25 C17:C18 E25 E17:E18 G25 G17:G18 I25 I17:I18 L25 L17:L18 I32 I34 L32 L34 G32 G34 E32 E34 C32 C34">
-    <cfRule type="cellIs" dxfId="95" priority="178" operator="greaterThan">
+  <conditionalFormatting sqref="C2:J3 C28:C29 I28:I29 L2:M3 E28:E29 G28:G29 L28:L29 L8:L13 G8:G13 E8:E13 C8:C13 L20 I20 G20 E20 C20 C4:C5 E4:E5 G4:G5 I4:I5 L4:L5 C25 C17:C18 E25 E17:E18 G25 G17:G18 I17:I18 L25 L17:L18 I32 I34 L32 L34 G32 G34 E32 E34 C32 C34 I8:I11 I13 I25">
+    <cfRule type="cellIs" dxfId="96" priority="178" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:M10 C27:M29 C20:M20 C2:M5 C25:M25 C17:M18 L34:M34 C32:M32 C34:J34 C12:M13 C11 E11:M11">
-    <cfRule type="cellIs" dxfId="94" priority="179" operator="greaterThan">
+  <conditionalFormatting sqref="C8:M10 C27:M29 C20:M20 C2:M5 C17:M18 L34:M34 C32:M32 C34:J34 C11 E11:M11 C13:M13 C12:G12 J12:M12 C25:M25">
+    <cfRule type="cellIs" dxfId="95" priority="179" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L27 I27 G27 E27 C27">
-    <cfRule type="cellIs" dxfId="93" priority="180" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="94" priority="180" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:J27 L27:M27">
-    <cfRule type="cellIs" dxfId="92" priority="181" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="93" priority="181" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32 F32 H32 J32 M32">
-    <cfRule type="cellIs" dxfId="91" priority="182" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="92" priority="182" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:M10 C27:M29 C20:M20 C2:M5 C25:M25 C17:M18 L34:M34 C32:M32 C34:J34 C12:M13 C11 E11:M11">
-    <cfRule type="cellIs" dxfId="90" priority="183" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8:M10 C27:M29 C20:M20 C2:M5 C25:M25 C17:M18 L34:M34 C32:M32 C34:J34 C12:M13 C11 E11:M11">
-    <cfRule type="cellIs" dxfId="89" priority="184" operator="greaterThan">
+  <conditionalFormatting sqref="C8:M10 C27:M29 C20:M20 C2:M5 C17:M18 L34:M34 C32:M32 C34:J34 C11 E11:M11 C13:M13 C12:G12 J12:M12 C25:M25">
+    <cfRule type="cellIs" dxfId="91" priority="183" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8:M10 C27:M29 C20:M20 C2:M5 C17:M18 L34:M34 C32:M32 C34:J34 C11 E11:M11 C13:M13 C12:G12 J12:M12 C25:M25">
+    <cfRule type="cellIs" dxfId="90" priority="184" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K3">
-    <cfRule type="cellIs" dxfId="88" priority="174" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="89" priority="174" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K3 K9:K13 K28:K29 K18 K32">
-    <cfRule type="cellIs" dxfId="87" priority="175" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="88" priority="175" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K27">
-    <cfRule type="cellIs" dxfId="86" priority="176" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="87" priority="176" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="85" priority="177" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="86" priority="177" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3 N27:N29 N5 N20 N22:N23 N8:N13 N25 N32 N34 N15:N18">
-    <cfRule type="cellIs" dxfId="84" priority="173" operator="equal">
+  <conditionalFormatting sqref="N3 N27:N29 N5 N20 N8:N13 N25 N32 N34 N15:N18 N22:N23">
+    <cfRule type="cellIs" dxfId="1" priority="173" operator="equal">
       <formula>$B3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="83" priority="172" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="172" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35:M35">
-    <cfRule type="cellIs" dxfId="82" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="171" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34">
-    <cfRule type="cellIs" dxfId="81" priority="170" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="83" priority="170" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F34">
-    <cfRule type="cellIs" dxfId="80" priority="169" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="82" priority="169" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="cellIs" dxfId="79" priority="168" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="81" priority="168" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J34">
-    <cfRule type="cellIs" dxfId="78" priority="167" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="80" priority="167" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K34">
-    <cfRule type="cellIs" dxfId="77" priority="162" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="79" priority="162" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K34">
-    <cfRule type="cellIs" dxfId="76" priority="163" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="78" priority="163" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K34">
-    <cfRule type="cellIs" dxfId="75" priority="164" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="77" priority="164" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K34">
-    <cfRule type="cellIs" dxfId="74" priority="165" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="76" priority="165" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K34">
-    <cfRule type="cellIs" dxfId="73" priority="166" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="75" priority="166" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M34">
-    <cfRule type="cellIs" dxfId="72" priority="161" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="74" priority="161" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2">
-    <cfRule type="cellIs" dxfId="71" priority="160" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="160" operator="equal">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4">
-    <cfRule type="cellIs" dxfId="70" priority="159" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="159" operator="equal">
       <formula>$B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7 E7 G7 I7 L7">
-    <cfRule type="cellIs" dxfId="69" priority="155" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="71" priority="155" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:J7 L7:M7">
-    <cfRule type="cellIs" dxfId="68" priority="156" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="70" priority="156" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:J7 L7:M7">
-    <cfRule type="cellIs" dxfId="67" priority="157" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="69" priority="157" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:J7 L7:M7">
-    <cfRule type="cellIs" dxfId="66" priority="158" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="68" priority="158" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="65" priority="152" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="67" priority="152" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="64" priority="153" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="66" priority="153" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="63" priority="154" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="65" priority="154" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K19">
-    <cfRule type="cellIs" dxfId="62" priority="145" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="64" priority="145" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19 E19 G19 I19 L19">
-    <cfRule type="cellIs" dxfId="61" priority="148" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="63" priority="148" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:J19 L19:M19">
-    <cfRule type="cellIs" dxfId="60" priority="149" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="62" priority="149" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:J19 L19:M19">
-    <cfRule type="cellIs" dxfId="59" priority="150" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="61" priority="150" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:J19 L19:M19">
-    <cfRule type="cellIs" dxfId="58" priority="151" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="60" priority="151" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K19">
-    <cfRule type="cellIs" dxfId="57" priority="146" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="59" priority="146" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K19">
-    <cfRule type="cellIs" dxfId="56" priority="147" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="58" priority="147" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L22:L23 I22:I23 G22:G23 E22:E23 C22:C23">
-    <cfRule type="cellIs" dxfId="55" priority="141" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="57" priority="141" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:M23">
-    <cfRule type="cellIs" dxfId="54" priority="142" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="56" priority="142" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:M23">
-    <cfRule type="cellIs" dxfId="53" priority="143" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="55" priority="143" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:M23">
-    <cfRule type="cellIs" dxfId="52" priority="144" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="54" priority="144" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22:K23">
-    <cfRule type="cellIs" dxfId="51" priority="140" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="53" priority="140" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21">
-    <cfRule type="cellIs" dxfId="50" priority="133" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="52" priority="133" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="cellIs" dxfId="49" priority="121" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="51" priority="121" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21 E21 G21 I21 L21">
-    <cfRule type="cellIs" dxfId="48" priority="136" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="50" priority="136" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:J21 L21:M21">
-    <cfRule type="cellIs" dxfId="47" priority="137" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="49" priority="137" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:J21 L21:M21">
-    <cfRule type="cellIs" dxfId="46" priority="138" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="48" priority="138" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:J21 L21:M21">
-    <cfRule type="cellIs" dxfId="45" priority="139" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="47" priority="139" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21">
-    <cfRule type="cellIs" dxfId="44" priority="134" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="134" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21">
-    <cfRule type="cellIs" dxfId="43" priority="135" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="135" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L15:L16 I15:I16 G15:G16 E15:E16 C15:C16">
-    <cfRule type="cellIs" dxfId="42" priority="129" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="44" priority="129" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:M16">
-    <cfRule type="cellIs" dxfId="41" priority="130" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="130" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:M16">
-    <cfRule type="cellIs" dxfId="40" priority="131" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="131" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:M16">
-    <cfRule type="cellIs" dxfId="39" priority="132" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="132" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15:K16">
-    <cfRule type="cellIs" dxfId="38" priority="128" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="40" priority="128" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30 E30 G30 I30 L30">
-    <cfRule type="cellIs" dxfId="37" priority="124" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="124" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:J30 L30:M30">
-    <cfRule type="cellIs" dxfId="36" priority="125" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="38" priority="125" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:J30 L30:M30">
-    <cfRule type="cellIs" dxfId="35" priority="126" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="126" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:J30 L30:M30">
-    <cfRule type="cellIs" dxfId="34" priority="127" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="127" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="cellIs" dxfId="33" priority="122" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="122" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="cellIs" dxfId="32" priority="123" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="123" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26 E26 G26 I26 L26">
-    <cfRule type="cellIs" dxfId="31" priority="117" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="117" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:J26 L26:M26">
-    <cfRule type="cellIs" dxfId="30" priority="118" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="118" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:J26 L26:M26">
-    <cfRule type="cellIs" dxfId="29" priority="119" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="119" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:J26 L26:M26">
-    <cfRule type="cellIs" dxfId="28" priority="120" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="120" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26">
-    <cfRule type="cellIs" dxfId="27" priority="114" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="114" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26">
-    <cfRule type="cellIs" dxfId="26" priority="115" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="115" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26">
-    <cfRule type="cellIs" dxfId="25" priority="116" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="116" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L32">
-    <cfRule type="cellIs" dxfId="24" priority="101" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="101" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I31 L31 G31 E31 C31">
-    <cfRule type="cellIs" dxfId="23" priority="109" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="109" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31:M31">
-    <cfRule type="cellIs" dxfId="22" priority="110" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="110" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31 F31 H31 J31 M31">
-    <cfRule type="cellIs" dxfId="21" priority="111" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="111" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31:M31">
-    <cfRule type="cellIs" dxfId="20" priority="112" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="112" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31:M31">
-    <cfRule type="cellIs" dxfId="19" priority="113" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="113" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31">
-    <cfRule type="cellIs" dxfId="18" priority="107" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="107" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31">
-    <cfRule type="cellIs" dxfId="17" priority="108" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="108" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N31">
-    <cfRule type="cellIs" dxfId="16" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="106" operator="equal">
       <formula>$B31</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="cellIs" dxfId="15" priority="105" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="105" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32">
-    <cfRule type="cellIs" dxfId="14" priority="104" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="104" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I32">
-    <cfRule type="cellIs" dxfId="13" priority="103" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="103" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="12" priority="102" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="102" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6 G6 I6 L6">
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="9" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:M6">
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:M6">
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:M6">
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14 I14 L14">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14:M14">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14:M14">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14:M14">
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L24">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J24:M24">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J24:M24">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J24:M24">
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
docs: documentation du jour 8, ajout de code source et du début du manuel utilisateur
</commit_message>
<xml_diff>
--- a/docs/plannification_TPI.xlsx
+++ b/docs/plannification_TPI.xlsx
@@ -578,7 +578,135 @@
     <cellStyle name="Insatisfaisant" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="189">
+  <dxfs count="188">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -590,6 +718,430 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
@@ -601,25 +1153,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -658,30 +1196,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFC6D9F0"/>
           <bgColor rgb="FFC6D9F0"/>
         </patternFill>
@@ -734,530 +1248,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4626,462 +4616,462 @@
     <mergeCell ref="A14:F14"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:J3 C26:C27 I26:I27 L2:M3 E26:E27 G26:G27 L26:L27 L8:L13 I8:I13 G8:G13 E8:E13 C8:C13 L19 I19 G19 E19 C19 C4:C5 E4:E6 G4:G6 I4:I6 L4:L6 C23 C16:C17 E23 E16:E17 G23 G16:G17 I23 I16:I17 L23 L16:L17 I30 I32 L30 L32 G30 G32 E30 E32 C30 C32">
-    <cfRule type="cellIs" dxfId="188" priority="194" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="187" priority="194" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:M13 C25:M27 C19:M19 C2:M5 C23:M23 C16:M17 D6:M6 L32:M32 C30:M30 C32:J32">
-    <cfRule type="cellIs" dxfId="187" priority="195" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="186" priority="195" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L25 I25 G25 E25 C25">
-    <cfRule type="cellIs" dxfId="186" priority="196" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="185" priority="196" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:J25 L25:M25">
-    <cfRule type="cellIs" dxfId="185" priority="197" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="184" priority="197" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30 F30 H30 J30 M30">
-    <cfRule type="cellIs" dxfId="184" priority="198" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="183" priority="198" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:M13 C25:M27 C19:M19 C2:M5 C23:M23 C16:M17 D6:M6 L32:M32 C30:M30 C32:J32">
-    <cfRule type="cellIs" dxfId="183" priority="201" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="182" priority="201" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:M13 C25:M27 C19:M19 C2:M5 C23:M23 C16:M17 D6:M6 L32:M32 C30:M30 C32:J32">
-    <cfRule type="cellIs" dxfId="182" priority="202" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="181" priority="202" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K3">
-    <cfRule type="cellIs" dxfId="181" priority="186" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="180" priority="186" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K3 K9:K13 K26:K27 K17 K30">
-    <cfRule type="cellIs" dxfId="180" priority="187" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="179" priority="187" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K25">
-    <cfRule type="cellIs" dxfId="179" priority="188" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="178" priority="188" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="cellIs" dxfId="178" priority="189" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="177" priority="189" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3 N25:N27 N5 N19 N21 N8:N13 N15:N17 N23 N30 N32">
-    <cfRule type="cellIs" dxfId="177" priority="184" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="184" operator="equal">
       <formula>$B3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="cellIs" dxfId="176" priority="181" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="181" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33:M33">
-    <cfRule type="cellIs" dxfId="175" priority="180" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="180" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32">
-    <cfRule type="cellIs" dxfId="174" priority="177" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="173" priority="177" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F32">
-    <cfRule type="cellIs" dxfId="173" priority="176" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="172" priority="176" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="cellIs" dxfId="172" priority="175" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="171" priority="175" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J32">
-    <cfRule type="cellIs" dxfId="171" priority="174" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="170" priority="174" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="170" priority="169" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="169" priority="169" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="169" priority="170" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="168" priority="170" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="168" priority="171" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="167" priority="171" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="167" priority="172" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="166" priority="172" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="166" priority="173" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="165" priority="173" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M32">
-    <cfRule type="cellIs" dxfId="165" priority="168" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="164" priority="168" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2">
-    <cfRule type="cellIs" dxfId="164" priority="167" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="167" operator="equal">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4">
-    <cfRule type="cellIs" dxfId="163" priority="166" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="166" operator="equal">
       <formula>$B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7 E7 G7 I7 L7">
-    <cfRule type="cellIs" dxfId="162" priority="162" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="161" priority="162" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:J7 L7:M7">
-    <cfRule type="cellIs" dxfId="161" priority="163" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="160" priority="163" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:J7 L7:M7">
-    <cfRule type="cellIs" dxfId="160" priority="164" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="159" priority="164" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:J7 L7:M7">
-    <cfRule type="cellIs" dxfId="159" priority="165" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="158" priority="165" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="158" priority="159" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="157" priority="159" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="157" priority="160" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="156" priority="160" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="156" priority="161" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="155" priority="161" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="155" priority="152" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="154" priority="152" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18 E18 G18 I18 L18">
-    <cfRule type="cellIs" dxfId="154" priority="155" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="153" priority="155" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:J18 L18:M18">
-    <cfRule type="cellIs" dxfId="153" priority="156" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="152" priority="156" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:J18 L18:M18">
-    <cfRule type="cellIs" dxfId="152" priority="157" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="151" priority="157" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:J18 L18:M18">
-    <cfRule type="cellIs" dxfId="151" priority="158" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="150" priority="158" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="150" priority="153" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="149" priority="153" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="149" priority="154" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="148" priority="154" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L21 I21 G21 E21 C21">
-    <cfRule type="cellIs" dxfId="148" priority="143" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="147" priority="143" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:M21">
-    <cfRule type="cellIs" dxfId="147" priority="144" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="146" priority="144" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:M21">
-    <cfRule type="cellIs" dxfId="146" priority="145" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="145" priority="145" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:M21">
-    <cfRule type="cellIs" dxfId="145" priority="146" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="144" priority="146" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21">
-    <cfRule type="cellIs" dxfId="144" priority="142" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="143" priority="142" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="cellIs" dxfId="143" priority="134" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="142" priority="134" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28">
-    <cfRule type="cellIs" dxfId="142" priority="121" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="141" priority="121" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20 E20 G20 I20 L20">
-    <cfRule type="cellIs" dxfId="141" priority="137" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="140" priority="137" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:J20 L20:M20">
-    <cfRule type="cellIs" dxfId="140" priority="138" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="139" priority="138" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:J20 L20:M20">
-    <cfRule type="cellIs" dxfId="139" priority="139" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="138" priority="139" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:J20 L20:M20">
-    <cfRule type="cellIs" dxfId="138" priority="140" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="137" priority="140" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="cellIs" dxfId="137" priority="135" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="136" priority="135" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="cellIs" dxfId="136" priority="136" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="135" priority="136" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L15 I15 G15 E15 C15">
-    <cfRule type="cellIs" dxfId="135" priority="130" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="134" priority="130" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:M15">
-    <cfRule type="cellIs" dxfId="134" priority="131" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="133" priority="131" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:M15">
-    <cfRule type="cellIs" dxfId="133" priority="132" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="132" priority="132" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:M15">
-    <cfRule type="cellIs" dxfId="132" priority="133" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="131" priority="133" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="cellIs" dxfId="131" priority="129" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="130" priority="129" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28 E28 G28 I28 L28">
-    <cfRule type="cellIs" dxfId="130" priority="124" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="129" priority="124" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:J28 L28:M28">
-    <cfRule type="cellIs" dxfId="129" priority="125" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="128" priority="125" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:J28 L28:M28">
-    <cfRule type="cellIs" dxfId="128" priority="126" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="127" priority="126" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:J28 L28:M28">
-    <cfRule type="cellIs" dxfId="127" priority="127" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="126" priority="127" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28">
-    <cfRule type="cellIs" dxfId="126" priority="122" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="125" priority="122" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28">
-    <cfRule type="cellIs" dxfId="125" priority="123" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="124" priority="123" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24 E24 G24 I24 L24">
-    <cfRule type="cellIs" dxfId="124" priority="117" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="123" priority="117" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:J24 L24:M24">
-    <cfRule type="cellIs" dxfId="123" priority="118" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="122" priority="118" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:J24 L24:M24">
-    <cfRule type="cellIs" dxfId="122" priority="119" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="121" priority="119" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:J24 L24:M24">
-    <cfRule type="cellIs" dxfId="121" priority="120" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="120" priority="120" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="120" priority="114" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="119" priority="114" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="119" priority="115" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="118" priority="115" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="118" priority="116" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="117" priority="116" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L30">
-    <cfRule type="cellIs" dxfId="117" priority="101" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="116" priority="101" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I29 L29 G29 E29 C29">
-    <cfRule type="cellIs" dxfId="116" priority="109" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="115" priority="109" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29:M29">
-    <cfRule type="cellIs" dxfId="115" priority="110" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="114" priority="110" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29 F29 H29 J29 M29">
-    <cfRule type="cellIs" dxfId="114" priority="111" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="113" priority="111" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29:M29">
-    <cfRule type="cellIs" dxfId="113" priority="112" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="112" priority="112" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29:M29">
-    <cfRule type="cellIs" dxfId="112" priority="113" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="111" priority="113" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K29">
-    <cfRule type="cellIs" dxfId="111" priority="107" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="110" priority="107" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K29">
-    <cfRule type="cellIs" dxfId="110" priority="108" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="109" priority="108" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N29">
-    <cfRule type="cellIs" dxfId="109" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="106" operator="equal">
       <formula>$B29</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="cellIs" dxfId="108" priority="105" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="107" priority="105" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30">
-    <cfRule type="cellIs" dxfId="107" priority="104" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="106" priority="104" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30">
-    <cfRule type="cellIs" dxfId="106" priority="103" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="105" priority="103" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="cellIs" dxfId="105" priority="102" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="104" priority="102" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14 I14 L14">
-    <cfRule type="cellIs" dxfId="104" priority="81" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="103" priority="81" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14:M14">
-    <cfRule type="cellIs" dxfId="103" priority="82" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="102" priority="82" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14:M14">
-    <cfRule type="cellIs" dxfId="102" priority="83" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="101" priority="83" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14:M14">
-    <cfRule type="cellIs" dxfId="101" priority="84" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="100" priority="84" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L22">
-    <cfRule type="cellIs" dxfId="100" priority="57" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="99" priority="57" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:M22">
-    <cfRule type="cellIs" dxfId="99" priority="58" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="98" priority="58" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:M22">
-    <cfRule type="cellIs" dxfId="98" priority="59" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="97" priority="59" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:M22">
-    <cfRule type="cellIs" dxfId="97" priority="60" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="96" priority="60" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5095,7 +5085,7 @@
   <dimension ref="A1:AF1006"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P37" sqref="P37"/>
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5958,13 +5948,15 @@
       <c r="I25" s="25">
         <v>0.125</v>
       </c>
-      <c r="J25" s="26"/>
+      <c r="J25" s="26">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="K25" s="26"/>
       <c r="L25" s="28"/>
       <c r="M25" s="23"/>
       <c r="N25" s="6">
         <f>SUM(C25:M25)</f>
-        <v>0.20833333333333331</v>
+        <v>0.24999999999999997</v>
       </c>
       <c r="O25" s="11"/>
       <c r="P25" s="11"/>
@@ -6192,13 +6184,15 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="I31" s="25"/>
-      <c r="J31" s="25"/>
+      <c r="J31" s="25">
+        <v>2.7777777777777776E-2</v>
+      </c>
       <c r="K31" s="25"/>
       <c r="L31" s="25"/>
       <c r="M31" s="29"/>
       <c r="N31" s="6">
         <f>SUM(C31:M31)</f>
-        <v>0.14583333333333334</v>
+        <v>0.1736111111111111</v>
       </c>
       <c r="O31" s="11"/>
       <c r="P31" s="11"/>
@@ -6243,13 +6237,15 @@
       <c r="I32" s="25">
         <v>0.19444444444444445</v>
       </c>
-      <c r="J32" s="25"/>
+      <c r="J32" s="25">
+        <v>0.25</v>
+      </c>
       <c r="K32" s="25"/>
       <c r="L32" s="39"/>
       <c r="M32" s="40"/>
       <c r="N32" s="6">
         <f>SUM(C32:M32)</f>
-        <v>0.54166666666666663</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="O32" s="11"/>
       <c r="P32" s="11"/>
@@ -6315,13 +6311,15 @@
       <c r="I34" s="31">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="J34" s="31"/>
+      <c r="J34" s="31">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="K34" s="31"/>
       <c r="L34" s="31"/>
       <c r="M34" s="41"/>
       <c r="N34" s="6">
         <f>SUM(C34:M34)</f>
-        <v>9.7222222222222238E-2</v>
+        <v>0.11111111111111113</v>
       </c>
       <c r="O34" s="11"/>
       <c r="P34" s="11"/>
@@ -6377,7 +6375,7 @@
       </c>
       <c r="J35" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="K35" s="6">
         <f t="shared" si="1"/>
@@ -6393,7 +6391,7 @@
       </c>
       <c r="N35" s="6">
         <f t="shared" si="1"/>
-        <v>2.333333333333333</v>
+        <v>2.6666666666666665</v>
       </c>
       <c r="O35" s="11"/>
       <c r="P35" s="11"/>
@@ -6417,7 +6415,7 @@
     <row r="36" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M36" s="42">
         <f>SUM(C35:M35)</f>
-        <v>2.3333333333333335</v>
+        <v>2.666666666666667</v>
       </c>
     </row>
     <row r="37" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -7420,482 +7418,482 @@
     <mergeCell ref="A33:M33"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:J3 C28:C29 I28:I29 L2:M3 E28:E29 G28:G29 L28:L29 L8:L13 G8:G13 E8:E13 C8:C13 L20 I20 G20 E20 C20 C4:C5 E4:E5 G4:G5 I4:I5 L4:L5 C25 C17:C18 E25 E17:E18 G25 G17:G18 I17:I18 L25 L17:L18 I32 I34 L32 L34 G32 G34 E32 E34 C32 C34 I8:I11 I13 I25">
-    <cfRule type="cellIs" dxfId="96" priority="178" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="95" priority="178" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:M10 C27:M29 C20:M20 C2:M5 C17:M18 L34:M34 C32:M32 C34:J34 C11 E11:M11 C13:M13 C12:G12 J12:M12 C25:M25">
-    <cfRule type="cellIs" dxfId="95" priority="179" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="94" priority="179" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L27 I27 G27 E27 C27">
-    <cfRule type="cellIs" dxfId="94" priority="180" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="93" priority="180" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:J27 L27:M27">
-    <cfRule type="cellIs" dxfId="93" priority="181" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="92" priority="181" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32 F32 H32 J32 M32">
-    <cfRule type="cellIs" dxfId="92" priority="182" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="91" priority="182" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:M10 C27:M29 C20:M20 C2:M5 C17:M18 L34:M34 C32:M32 C34:J34 C11 E11:M11 C13:M13 C12:G12 J12:M12 C25:M25">
-    <cfRule type="cellIs" dxfId="91" priority="183" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="90" priority="183" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:M10 C27:M29 C20:M20 C2:M5 C17:M18 L34:M34 C32:M32 C34:J34 C11 E11:M11 C13:M13 C12:G12 J12:M12 C25:M25">
-    <cfRule type="cellIs" dxfId="90" priority="184" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="89" priority="184" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K3">
-    <cfRule type="cellIs" dxfId="89" priority="174" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="88" priority="174" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K3 K9:K13 K28:K29 K18 K32">
-    <cfRule type="cellIs" dxfId="88" priority="175" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="87" priority="175" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K27">
-    <cfRule type="cellIs" dxfId="87" priority="176" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="86" priority="176" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="86" priority="177" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="85" priority="177" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3 N27:N29 N5 N20 N8:N13 N25 N32 N34 N15:N18 N22:N23">
-    <cfRule type="cellIs" dxfId="1" priority="173" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="173" operator="equal">
       <formula>$B3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="85" priority="172" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="172" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35:M35">
-    <cfRule type="cellIs" dxfId="84" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="171" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34">
-    <cfRule type="cellIs" dxfId="83" priority="170" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="81" priority="170" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F34">
-    <cfRule type="cellIs" dxfId="82" priority="169" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="80" priority="169" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="cellIs" dxfId="81" priority="168" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="79" priority="168" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J34">
-    <cfRule type="cellIs" dxfId="80" priority="167" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="78" priority="167" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K34">
-    <cfRule type="cellIs" dxfId="79" priority="162" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="77" priority="162" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K34">
-    <cfRule type="cellIs" dxfId="78" priority="163" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="76" priority="163" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K34">
-    <cfRule type="cellIs" dxfId="77" priority="164" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="75" priority="164" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K34">
-    <cfRule type="cellIs" dxfId="76" priority="165" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="74" priority="165" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K34">
-    <cfRule type="cellIs" dxfId="75" priority="166" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="73" priority="166" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M34">
-    <cfRule type="cellIs" dxfId="74" priority="161" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="72" priority="161" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2">
-    <cfRule type="cellIs" dxfId="73" priority="160" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="160" operator="equal">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4">
-    <cfRule type="cellIs" dxfId="72" priority="159" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="159" operator="equal">
       <formula>$B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7 E7 G7 I7 L7">
-    <cfRule type="cellIs" dxfId="71" priority="155" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="69" priority="155" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:J7 L7:M7">
-    <cfRule type="cellIs" dxfId="70" priority="156" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="68" priority="156" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:J7 L7:M7">
-    <cfRule type="cellIs" dxfId="69" priority="157" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="67" priority="157" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:J7 L7:M7">
-    <cfRule type="cellIs" dxfId="68" priority="158" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="66" priority="158" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="67" priority="152" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="65" priority="152" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="66" priority="153" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="64" priority="153" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="65" priority="154" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="63" priority="154" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K19">
-    <cfRule type="cellIs" dxfId="64" priority="145" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="62" priority="145" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19 E19 G19 I19 L19">
-    <cfRule type="cellIs" dxfId="63" priority="148" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="61" priority="148" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:J19 L19:M19">
-    <cfRule type="cellIs" dxfId="62" priority="149" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="60" priority="149" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:J19 L19:M19">
-    <cfRule type="cellIs" dxfId="61" priority="150" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="59" priority="150" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:J19 L19:M19">
-    <cfRule type="cellIs" dxfId="60" priority="151" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="58" priority="151" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K19">
-    <cfRule type="cellIs" dxfId="59" priority="146" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="57" priority="146" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K19">
-    <cfRule type="cellIs" dxfId="58" priority="147" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="56" priority="147" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L22:L23 I22:I23 G22:G23 E22:E23 C22:C23">
-    <cfRule type="cellIs" dxfId="57" priority="141" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="55" priority="141" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:M23">
-    <cfRule type="cellIs" dxfId="56" priority="142" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="54" priority="142" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:M23">
-    <cfRule type="cellIs" dxfId="55" priority="143" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="53" priority="143" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:M23">
-    <cfRule type="cellIs" dxfId="54" priority="144" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="52" priority="144" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22:K23">
-    <cfRule type="cellIs" dxfId="53" priority="140" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="51" priority="140" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21">
-    <cfRule type="cellIs" dxfId="52" priority="133" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="50" priority="133" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="cellIs" dxfId="51" priority="121" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="49" priority="121" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21 E21 G21 I21 L21">
-    <cfRule type="cellIs" dxfId="50" priority="136" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="48" priority="136" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:J21 L21:M21">
-    <cfRule type="cellIs" dxfId="49" priority="137" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="47" priority="137" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:J21 L21:M21">
-    <cfRule type="cellIs" dxfId="48" priority="138" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="138" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:J21 L21:M21">
-    <cfRule type="cellIs" dxfId="47" priority="139" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="139" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21">
-    <cfRule type="cellIs" dxfId="46" priority="134" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="44" priority="134" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21">
-    <cfRule type="cellIs" dxfId="45" priority="135" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="135" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L15:L16 I15:I16 G15:G16 E15:E16 C15:C16">
-    <cfRule type="cellIs" dxfId="44" priority="129" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="129" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:M16">
-    <cfRule type="cellIs" dxfId="43" priority="130" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="130" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:M16">
-    <cfRule type="cellIs" dxfId="42" priority="131" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="40" priority="131" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:M16">
-    <cfRule type="cellIs" dxfId="41" priority="132" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="132" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15:K16">
-    <cfRule type="cellIs" dxfId="40" priority="128" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="38" priority="128" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30 E30 G30 I30 L30">
-    <cfRule type="cellIs" dxfId="39" priority="124" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="124" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:J30 L30:M30">
-    <cfRule type="cellIs" dxfId="38" priority="125" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="125" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:J30 L30:M30">
-    <cfRule type="cellIs" dxfId="37" priority="126" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="126" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:J30 L30:M30">
-    <cfRule type="cellIs" dxfId="36" priority="127" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="127" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="cellIs" dxfId="35" priority="122" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="122" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="cellIs" dxfId="34" priority="123" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="123" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26 E26 G26 I26 L26">
-    <cfRule type="cellIs" dxfId="33" priority="117" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="117" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:J26 L26:M26">
-    <cfRule type="cellIs" dxfId="32" priority="118" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="118" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:J26 L26:M26">
-    <cfRule type="cellIs" dxfId="31" priority="119" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="119" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:J26 L26:M26">
-    <cfRule type="cellIs" dxfId="30" priority="120" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="120" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26">
-    <cfRule type="cellIs" dxfId="29" priority="114" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="114" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26">
-    <cfRule type="cellIs" dxfId="28" priority="115" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="115" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26">
-    <cfRule type="cellIs" dxfId="27" priority="116" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="116" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L32">
-    <cfRule type="cellIs" dxfId="26" priority="101" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="101" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I31 L31 G31 E31 C31">
-    <cfRule type="cellIs" dxfId="25" priority="109" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="109" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31:M31">
-    <cfRule type="cellIs" dxfId="24" priority="110" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="110" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31 F31 H31 J31 M31">
-    <cfRule type="cellIs" dxfId="23" priority="111" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="111" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31:M31">
-    <cfRule type="cellIs" dxfId="22" priority="112" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="112" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31:M31">
-    <cfRule type="cellIs" dxfId="21" priority="113" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="113" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31">
-    <cfRule type="cellIs" dxfId="20" priority="107" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="107" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31">
-    <cfRule type="cellIs" dxfId="19" priority="108" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="108" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N31">
-    <cfRule type="cellIs" dxfId="18" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="106" operator="equal">
       <formula>$B31</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="cellIs" dxfId="17" priority="105" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="105" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32">
-    <cfRule type="cellIs" dxfId="16" priority="104" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="104" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I32">
-    <cfRule type="cellIs" dxfId="15" priority="103" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="103" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="14" priority="102" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="102" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6 G6 I6 L6">
-    <cfRule type="cellIs" dxfId="13" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:M6">
-    <cfRule type="cellIs" dxfId="12" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:M6">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:M6">
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14 I14 L14">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14:M14">
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14:M14">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14:M14">
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L24">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J24:M24">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J24:M24">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J24:M24">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
docs: documentation du jour 9
</commit_message>
<xml_diff>
--- a/docs/plannification_TPI.xlsx
+++ b/docs/plannification_TPI.xlsx
@@ -2321,7 +2321,7 @@
   <dimension ref="A1:AF1004"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="AA44" sqref="AA44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5085,7 +5085,7 @@
   <dimension ref="A1:AF1006"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5951,12 +5951,14 @@
       <c r="J25" s="26">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="K25" s="26"/>
+      <c r="K25" s="26">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="L25" s="28"/>
       <c r="M25" s="23"/>
       <c r="N25" s="6">
         <f>SUM(C25:M25)</f>
-        <v>0.24999999999999997</v>
+        <v>0.27083333333333331</v>
       </c>
       <c r="O25" s="11"/>
       <c r="P25" s="11"/>
@@ -6240,12 +6242,14 @@
       <c r="J32" s="25">
         <v>0.25</v>
       </c>
-      <c r="K32" s="25"/>
+      <c r="K32" s="25">
+        <v>0.2986111111111111</v>
+      </c>
       <c r="L32" s="39"/>
       <c r="M32" s="40"/>
       <c r="N32" s="6">
         <f>SUM(C32:M32)</f>
-        <v>0.79166666666666663</v>
+        <v>1.0902777777777777</v>
       </c>
       <c r="O32" s="11"/>
       <c r="P32" s="11"/>
@@ -6314,12 +6318,14 @@
       <c r="J34" s="31">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="K34" s="31"/>
+      <c r="K34" s="31">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="L34" s="31"/>
       <c r="M34" s="41"/>
       <c r="N34" s="6">
         <f>SUM(C34:M34)</f>
-        <v>0.11111111111111113</v>
+        <v>0.12500000000000003</v>
       </c>
       <c r="O34" s="11"/>
       <c r="P34" s="11"/>
@@ -6379,7 +6385,7 @@
       </c>
       <c r="K35" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="L35" s="6">
         <f t="shared" si="1"/>
@@ -6391,7 +6397,7 @@
       </c>
       <c r="N35" s="6">
         <f t="shared" si="1"/>
-        <v>2.6666666666666665</v>
+        <v>3</v>
       </c>
       <c r="O35" s="11"/>
       <c r="P35" s="11"/>
@@ -6415,7 +6421,7 @@
     <row r="36" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M36" s="42">
         <f>SUM(C35:M35)</f>
-        <v>2.666666666666667</v>
+        <v>3.0000000000000004</v>
       </c>
     </row>
     <row r="37" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
docs: documentation du jour 11
</commit_message>
<xml_diff>
--- a/docs/plannification_TPI.xlsx
+++ b/docs/plannification_TPI.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="37">
   <si>
     <t>Tâches à réaliser</t>
   </si>
@@ -147,9 +147,6 @@
   <si>
     <t>Temps prévu</t>
   </si>
-  <si>
-    <t>Commentaire / refactorisation</t>
-  </si>
 </sst>
 </file>
 
@@ -159,7 +156,7 @@
     <numFmt numFmtId="164" formatCode="[hh]:mm"/>
     <numFmt numFmtId="165" formatCode="dd/mm"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,8 +212,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -238,6 +242,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -440,11 +449,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -573,10 +583,14 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Insatisfaisant" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Satisfaisant" xfId="2" builtinId="26"/>
   </cellStyles>
   <dxfs count="188">
     <dxf>
@@ -5082,10 +5096,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF1006"/>
+  <dimension ref="A1:AF1005"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5365,7 +5379,7 @@
       <c r="K8" s="22"/>
       <c r="L8" s="18"/>
       <c r="M8" s="23"/>
-      <c r="N8" s="6">
+      <c r="N8" s="50">
         <f t="shared" ref="N8:N13" si="0">SUM(C8:M8)</f>
         <v>2.0833333333333332E-2</v>
       </c>
@@ -5408,7 +5422,7 @@
       <c r="K9" s="26"/>
       <c r="L9" s="25"/>
       <c r="M9" s="27"/>
-      <c r="N9" s="6">
+      <c r="N9" s="50">
         <f t="shared" si="0"/>
         <v>1.3888888888888888E-2</v>
       </c>
@@ -5451,7 +5465,7 @@
       <c r="K10" s="26"/>
       <c r="L10" s="25"/>
       <c r="M10" s="27"/>
-      <c r="N10" s="6">
+      <c r="N10" s="50">
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
@@ -5535,7 +5549,7 @@
       <c r="K12" s="26"/>
       <c r="L12" s="25"/>
       <c r="M12" s="27"/>
-      <c r="N12" s="6">
+      <c r="N12" s="45">
         <f t="shared" si="0"/>
         <v>0.27083333333333331</v>
       </c>
@@ -5578,7 +5592,7 @@
       <c r="K13" s="26"/>
       <c r="L13" s="28"/>
       <c r="M13" s="27"/>
-      <c r="N13" s="6">
+      <c r="N13" s="50">
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
@@ -5656,7 +5670,7 @@
       <c r="K15" s="26"/>
       <c r="L15" s="28"/>
       <c r="M15" s="27"/>
-      <c r="N15" s="6">
+      <c r="N15" s="50">
         <f>SUM(C15:M15)</f>
         <v>0.19444444444444445</v>
       </c>
@@ -5699,7 +5713,7 @@
       <c r="K16" s="26"/>
       <c r="L16" s="28"/>
       <c r="M16" s="23"/>
-      <c r="N16" s="6">
+      <c r="N16" s="50">
         <f>SUM(C16:M16)</f>
         <v>6.25E-2</v>
       </c>
@@ -5738,11 +5752,13 @@
       <c r="I17" s="18"/>
       <c r="J17" s="22"/>
       <c r="K17" s="22"/>
-      <c r="L17" s="18"/>
+      <c r="L17" s="18">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="M17" s="23"/>
-      <c r="N17" s="6">
+      <c r="N17" s="50">
         <f>SUM(C17:M17)</f>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="18" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -5885,81 +5901,93 @@
       <c r="K22" s="26"/>
       <c r="L22" s="28"/>
       <c r="M22" s="27"/>
-      <c r="N22" s="6">
+      <c r="N22" s="50">
         <f>SUM(C22:M22)</f>
         <v>9.0277777777777776E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="24"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="26">
+    <row r="23" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="48"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="23"/>
+    </row>
+    <row r="24" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="17">
+        <v>0.2986111111111111</v>
+      </c>
+      <c r="C24" s="28"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="26">
+        <v>0.125</v>
+      </c>
+      <c r="I24" s="25">
+        <v>0.125</v>
+      </c>
+      <c r="J24" s="26">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="I23" s="25"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="28"/>
-      <c r="M23" s="23"/>
-      <c r="N23" s="6">
-        <f>SUM(C23:M23)</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
+      <c r="K24" s="26">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="L24" s="28"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="6">
+        <f>SUM(C24:M24)</f>
+        <v>0.3125</v>
+      </c>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="11"/>
+      <c r="U24" s="11"/>
+      <c r="V24" s="11"/>
+      <c r="W24" s="11"/>
+      <c r="X24" s="11"/>
+      <c r="Y24" s="11"/>
+      <c r="Z24" s="11"/>
+      <c r="AA24" s="11"/>
+      <c r="AB24" s="11"/>
+      <c r="AC24" s="11"/>
+      <c r="AD24" s="11"/>
+      <c r="AE24" s="11"/>
+      <c r="AF24" s="11"/>
     </row>
-    <row r="24" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="48"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="48"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="22"/>
-      <c r="L24" s="18"/>
-      <c r="M24" s="23"/>
-    </row>
-    <row r="25" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="17">
-        <v>0.2986111111111111</v>
-      </c>
-      <c r="C25" s="28"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="26">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="I25" s="25">
-        <v>0.125</v>
-      </c>
-      <c r="J25" s="26">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="K25" s="26">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="L25" s="28"/>
-      <c r="M25" s="23"/>
-      <c r="N25" s="6">
-        <f>SUM(C25:M25)</f>
-        <v>0.27083333333333331</v>
-      </c>
+    <row r="25" spans="1:32" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="5"/>
       <c r="O25" s="11"/>
       <c r="P25" s="11"/>
       <c r="Q25" s="11"/>
@@ -5979,22 +6007,26 @@
       <c r="AE25" s="11"/>
       <c r="AF25" s="11"/>
     </row>
-    <row r="26" spans="1:32" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="5"/>
+    <row r="26" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="24"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="25"/>
+      <c r="M26" s="27"/>
+      <c r="N26" s="6">
+        <f>SUM(C26:M26)</f>
+        <v>0</v>
+      </c>
       <c r="O26" s="11"/>
       <c r="P26" s="11"/>
       <c r="Q26" s="11"/>
@@ -6016,7 +6048,7 @@
     </row>
     <row r="27" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B27" s="24"/>
       <c r="C27" s="25"/>
@@ -6055,14 +6087,14 @@
     </row>
     <row r="28" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="35" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B28" s="24"/>
-      <c r="C28" s="25"/>
+      <c r="C28" s="28"/>
       <c r="D28" s="26"/>
-      <c r="E28" s="25"/>
+      <c r="E28" s="28"/>
       <c r="F28" s="26"/>
-      <c r="G28" s="25"/>
+      <c r="G28" s="28"/>
       <c r="H28" s="26"/>
       <c r="I28" s="25"/>
       <c r="J28" s="26"/>
@@ -6092,26 +6124,22 @@
       <c r="AE28" s="11"/>
       <c r="AF28" s="11"/>
     </row>
-    <row r="29" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" s="24"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="26"/>
-      <c r="K29" s="26"/>
-      <c r="L29" s="25"/>
-      <c r="M29" s="27"/>
-      <c r="N29" s="6">
-        <f>SUM(C29:M29)</f>
-        <v>0</v>
-      </c>
+    <row r="29" spans="1:32" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="5"/>
       <c r="O29" s="11"/>
       <c r="P29" s="11"/>
       <c r="Q29" s="11"/>
@@ -6131,22 +6159,36 @@
       <c r="AE29" s="11"/>
       <c r="AF29" s="11"/>
     </row>
-    <row r="30" spans="1:32" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="5"/>
+    <row r="30" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="C30" s="25">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="H30" s="25">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="I30" s="25"/>
+      <c r="J30" s="25">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="K30" s="25"/>
+      <c r="L30" s="25"/>
+      <c r="M30" s="29"/>
+      <c r="N30" s="6">
+        <f>SUM(C30:M30)</f>
+        <v>0.1736111111111111</v>
+      </c>
       <c r="O30" s="11"/>
       <c r="P30" s="11"/>
       <c r="Q30" s="11"/>
@@ -6167,34 +6209,42 @@
       <c r="AF30" s="11"/>
     </row>
     <row r="31" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="35" t="s">
-        <v>25</v>
+      <c r="A31" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="B31" s="24">
-        <v>0.5</v>
+        <v>1.0416666666666667</v>
       </c>
       <c r="C31" s="25">
-        <v>0.10416666666666667</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
+      <c r="E31" s="25">
+        <v>4.8611111111111112E-2</v>
+      </c>
       <c r="F31" s="25"/>
       <c r="G31" s="25">
-        <v>2.0833333333333332E-2</v>
+        <v>0.17361111111111113</v>
       </c>
       <c r="H31" s="25">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="I31" s="25"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="I31" s="25">
+        <v>0.19444444444444445</v>
+      </c>
       <c r="J31" s="25">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="K31" s="25"/>
-      <c r="L31" s="25"/>
-      <c r="M31" s="29"/>
+        <v>0.25</v>
+      </c>
+      <c r="K31" s="25">
+        <v>0.2986111111111111</v>
+      </c>
+      <c r="L31" s="39">
+        <v>0.2986111111111111</v>
+      </c>
+      <c r="M31" s="40"/>
       <c r="N31" s="6">
         <f>SUM(C31:M31)</f>
-        <v>0.1736111111111111</v>
+        <v>1.3888888888888888</v>
       </c>
       <c r="O31" s="11"/>
       <c r="P31" s="11"/>
@@ -6215,117 +6265,136 @@
       <c r="AE31" s="11"/>
       <c r="AF31" s="11"/>
     </row>
-    <row r="32" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" s="24">
-        <v>1.0416666666666667</v>
-      </c>
-      <c r="C32" s="25">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25">
-        <v>4.8611111111111112E-2</v>
-      </c>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25">
-        <v>0.17361111111111113</v>
-      </c>
-      <c r="H32" s="25">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="I32" s="25">
-        <v>0.19444444444444445</v>
-      </c>
-      <c r="J32" s="25">
-        <v>0.25</v>
-      </c>
-      <c r="K32" s="25">
-        <v>0.2986111111111111</v>
-      </c>
-      <c r="L32" s="39"/>
-      <c r="M32" s="40"/>
-      <c r="N32" s="6">
-        <f>SUM(C32:M32)</f>
-        <v>1.0902777777777777</v>
-      </c>
-      <c r="O32" s="11"/>
-      <c r="P32" s="11"/>
-      <c r="Q32" s="11"/>
-      <c r="R32" s="11"/>
-      <c r="S32" s="11"/>
-      <c r="T32" s="11"/>
-      <c r="U32" s="11"/>
-      <c r="V32" s="11"/>
-      <c r="W32" s="11"/>
-      <c r="X32" s="11"/>
-      <c r="Y32" s="11"/>
-      <c r="Z32" s="11"/>
-      <c r="AA32" s="11"/>
-      <c r="AB32" s="11"/>
-      <c r="AC32" s="11"/>
-      <c r="AD32" s="11"/>
-      <c r="AE32" s="11"/>
-      <c r="AF32" s="11"/>
+    <row r="32" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="48"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="48"/>
+      <c r="E32" s="48"/>
+      <c r="F32" s="48"/>
+      <c r="G32" s="48"/>
+      <c r="H32" s="48"/>
+      <c r="I32" s="48"/>
+      <c r="J32" s="48"/>
+      <c r="K32" s="48"/>
+      <c r="L32" s="48"/>
+      <c r="M32" s="49"/>
     </row>
-    <row r="33" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="48"/>
-      <c r="C33" s="48"/>
-      <c r="D33" s="48"/>
-      <c r="E33" s="48"/>
-      <c r="F33" s="48"/>
-      <c r="G33" s="48"/>
-      <c r="H33" s="48"/>
-      <c r="I33" s="48"/>
-      <c r="J33" s="48"/>
-      <c r="K33" s="48"/>
-      <c r="L33" s="48"/>
-      <c r="M33" s="49"/>
+    <row r="33" spans="1:32" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="30">
+        <v>0.15277777777777776</v>
+      </c>
+      <c r="C33" s="31">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="D33" s="31">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E33" s="31">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="F33" s="31">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="G33" s="31">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="H33" s="31">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="I33" s="31">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="J33" s="31">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="K33" s="31">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="L33" s="31">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="M33" s="41"/>
+      <c r="N33" s="6">
+        <f>SUM(C33:M33)</f>
+        <v>0.13888888888888892</v>
+      </c>
+      <c r="O33" s="11"/>
+      <c r="P33" s="11"/>
+      <c r="Q33" s="11"/>
+      <c r="R33" s="11"/>
+      <c r="S33" s="11"/>
+      <c r="T33" s="11"/>
+      <c r="U33" s="11"/>
+      <c r="V33" s="11"/>
+      <c r="W33" s="11"/>
+      <c r="X33" s="11"/>
+      <c r="Y33" s="11"/>
+      <c r="Z33" s="11"/>
+      <c r="AA33" s="11"/>
+      <c r="AB33" s="11"/>
+      <c r="AC33" s="11"/>
+      <c r="AD33" s="11"/>
+      <c r="AE33" s="11"/>
+      <c r="AF33" s="11"/>
     </row>
-    <row r="34" spans="1:32" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" s="30">
-        <v>0.15277777777777776</v>
-      </c>
-      <c r="C34" s="31">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="D34" s="31">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="E34" s="31">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="F34" s="31">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="G34" s="31">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="H34" s="31">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="I34" s="31">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="J34" s="31">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="K34" s="31">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="L34" s="31"/>
-      <c r="M34" s="41"/>
+    <row r="34" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="6">
+        <f t="shared" ref="B34:N34" si="1">SUM(B2:B33)</f>
+        <v>3.666666666666667</v>
+      </c>
+      <c r="C34" s="6">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="D34" s="6">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E34" s="6">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F34" s="6">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G34" s="6">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="H34" s="6">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="I34" s="6">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J34" s="6">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K34" s="6">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="L34" s="6">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M34" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="N34" s="6">
-        <f>SUM(C34:M34)</f>
-        <v>0.12500000000000003</v>
+        <f t="shared" si="1"/>
+        <v>3.333333333333333</v>
       </c>
       <c r="O34" s="11"/>
       <c r="P34" s="11"/>
@@ -6347,108 +6416,37 @@
       <c r="AF34" s="11"/>
     </row>
     <row r="35" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="6">
-        <f t="shared" ref="B35:N35" si="1">SUM(B2:B34)</f>
-        <v>3.666666666666667</v>
-      </c>
-      <c r="C35" s="6">
-        <f t="shared" si="1"/>
-        <v>0.33333333333333337</v>
-      </c>
-      <c r="D35" s="6">
-        <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="E35" s="6">
-        <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="F35" s="6">
-        <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="G35" s="6">
-        <f t="shared" si="1"/>
-        <v>0.33333333333333337</v>
-      </c>
-      <c r="H35" s="6">
-        <f t="shared" si="1"/>
-        <v>0.33333333333333337</v>
-      </c>
-      <c r="I35" s="6">
-        <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="J35" s="6">
-        <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="K35" s="6">
-        <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="L35" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M35" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N35" s="6">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="O35" s="11"/>
-      <c r="P35" s="11"/>
-      <c r="Q35" s="11"/>
-      <c r="R35" s="11"/>
-      <c r="S35" s="11"/>
-      <c r="T35" s="11"/>
-      <c r="U35" s="11"/>
-      <c r="V35" s="11"/>
-      <c r="W35" s="11"/>
-      <c r="X35" s="11"/>
-      <c r="Y35" s="11"/>
-      <c r="Z35" s="11"/>
-      <c r="AA35" s="11"/>
-      <c r="AB35" s="11"/>
-      <c r="AC35" s="11"/>
-      <c r="AD35" s="11"/>
-      <c r="AE35" s="11"/>
-      <c r="AF35" s="11"/>
+      <c r="M35" s="42">
+        <f>SUM(C34:M34)</f>
+        <v>3.3333333333333339</v>
+      </c>
     </row>
     <row r="36" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M36" s="42">
-        <f>SUM(C35:M35)</f>
-        <v>3.0000000000000004</v>
+      <c r="F36" s="44" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F37" s="44" t="s">
-        <v>28</v>
-      </c>
+      <c r="O37" s="11"/>
+      <c r="P37" s="11"/>
+      <c r="Q37" s="11"/>
+      <c r="R37" s="11"/>
+      <c r="S37" s="11"/>
+      <c r="T37" s="11"/>
+      <c r="U37" s="11"/>
+      <c r="V37" s="11"/>
+      <c r="W37" s="11"/>
+      <c r="X37" s="11"/>
+      <c r="Y37" s="11"/>
+      <c r="Z37" s="11"/>
+      <c r="AA37" s="11"/>
+      <c r="AB37" s="11"/>
+      <c r="AC37" s="11"/>
+      <c r="AD37" s="11"/>
+      <c r="AE37" s="11"/>
+      <c r="AF37" s="11"/>
     </row>
-    <row r="38" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="O38" s="11"/>
-      <c r="P38" s="11"/>
-      <c r="Q38" s="11"/>
-      <c r="R38" s="11"/>
-      <c r="S38" s="11"/>
-      <c r="T38" s="11"/>
-      <c r="U38" s="11"/>
-      <c r="V38" s="11"/>
-      <c r="W38" s="11"/>
-      <c r="X38" s="11"/>
-      <c r="Y38" s="11"/>
-      <c r="Z38" s="11"/>
-      <c r="AA38" s="11"/>
-      <c r="AB38" s="11"/>
-      <c r="AC38" s="11"/>
-      <c r="AD38" s="11"/>
-      <c r="AE38" s="11"/>
-      <c r="AF38" s="11"/>
-    </row>
+    <row r="39" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="40" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="41" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="42" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6465,7 +6463,7 @@
     <row r="53" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="54" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="55" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="59" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7415,45 +7413,44 @@
     <row r="1003" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1004" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1005" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1006" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A14:F14"/>
-    <mergeCell ref="A24:I24"/>
-    <mergeCell ref="A33:M33"/>
+    <mergeCell ref="A23:I23"/>
+    <mergeCell ref="A32:M32"/>
   </mergeCells>
-  <conditionalFormatting sqref="C2:J3 C28:C29 I28:I29 L2:M3 E28:E29 G28:G29 L28:L29 L8:L13 G8:G13 E8:E13 C8:C13 L20 I20 G20 E20 C20 C4:C5 E4:E5 G4:G5 I4:I5 L4:L5 C25 C17:C18 E25 E17:E18 G25 G17:G18 I17:I18 L25 L17:L18 I32 I34 L32 L34 G32 G34 E32 E34 C32 C34 I8:I11 I13 I25">
+  <conditionalFormatting sqref="C2:J3 C27:C28 I27:I28 L2:M3 E27:E28 G27:G28 L27:L28 L8:L13 G8:G13 E8:E13 C8:C13 L20 I20 G20 E20 C20 C4:C5 E4:E5 G4:G5 I4:I5 L4:L5 C24 C17:C18 E24 E17:E18 G24 G17:G18 I17:I18 L24 L17:L18 I31 I33 L31 L33 G31 G33 E31 E33 C31 C33 I8:I11 I13 I24">
     <cfRule type="cellIs" dxfId="95" priority="178" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:M10 C27:M29 C20:M20 C2:M5 C17:M18 L34:M34 C32:M32 C34:J34 C11 E11:M11 C13:M13 C12:G12 J12:M12 C25:M25">
+  <conditionalFormatting sqref="C8:M10 C26:M28 C20:M20 C2:M5 C17:M18 L33:M33 C31:M31 C33:J33 C11 E11:M11 C13:M13 C12:G12 J12:M12 C24:M24">
     <cfRule type="cellIs" dxfId="94" priority="179" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L27 I27 G27 E27 C27">
+  <conditionalFormatting sqref="L26 I26 G26 E26 C26">
     <cfRule type="cellIs" dxfId="93" priority="180" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C27:J27 L27:M27">
+  <conditionalFormatting sqref="C26:J26 L26:M26">
     <cfRule type="cellIs" dxfId="92" priority="181" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D32 F32 H32 J32 M32">
+  <conditionalFormatting sqref="D31 F31 H31 J31 M31">
     <cfRule type="cellIs" dxfId="91" priority="182" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:M10 C27:M29 C20:M20 C2:M5 C17:M18 L34:M34 C32:M32 C34:J34 C11 E11:M11 C13:M13 C12:G12 J12:M12 C25:M25">
+  <conditionalFormatting sqref="C8:M10 C26:M28 C20:M20 C2:M5 C17:M18 L33:M33 C31:M31 C33:J33 C11 E11:M11 C13:M13 C12:G12 J12:M12 C24:M24">
     <cfRule type="cellIs" dxfId="90" priority="183" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:M10 C27:M29 C20:M20 C2:M5 C17:M18 L34:M34 C32:M32 C34:J34 C11 E11:M11 C13:M13 C12:G12 J12:M12 C25:M25">
+  <conditionalFormatting sqref="C8:M10 C26:M28 C20:M20 C2:M5 C17:M18 L33:M33 C31:M31 C33:J33 C11 E11:M11 C13:M13 C12:G12 J12:M12 C24:M24">
     <cfRule type="cellIs" dxfId="89" priority="184" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7463,82 +7460,82 @@
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K3 K9:K13 K28:K29 K18 K32">
+  <conditionalFormatting sqref="K2:K3 K9:K13 K27:K28 K18 K31">
     <cfRule type="cellIs" dxfId="87" priority="175" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K27">
+  <conditionalFormatting sqref="K26">
     <cfRule type="cellIs" dxfId="86" priority="176" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K32">
+  <conditionalFormatting sqref="K31">
     <cfRule type="cellIs" dxfId="85" priority="177" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3 N27:N29 N5 N20 N8:N13 N25 N32 N34 N15:N18 N22:N23">
+  <conditionalFormatting sqref="N3 N26:N28 N5 N20 N8:N13 N24 N31 N33 N15:N18 N22">
     <cfRule type="cellIs" dxfId="84" priority="173" operator="equal">
       <formula>$B3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+  <conditionalFormatting sqref="C34">
     <cfRule type="cellIs" dxfId="83" priority="172" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D35:M35">
+  <conditionalFormatting sqref="D34:M34">
     <cfRule type="cellIs" dxfId="82" priority="171" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
+  <conditionalFormatting sqref="D33">
     <cfRule type="cellIs" dxfId="81" priority="170" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F34">
+  <conditionalFormatting sqref="F33">
     <cfRule type="cellIs" dxfId="80" priority="169" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H34">
+  <conditionalFormatting sqref="H33">
     <cfRule type="cellIs" dxfId="79" priority="168" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J34">
+  <conditionalFormatting sqref="J33">
     <cfRule type="cellIs" dxfId="78" priority="167" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K34">
+  <conditionalFormatting sqref="K33">
     <cfRule type="cellIs" dxfId="77" priority="162" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K34">
+  <conditionalFormatting sqref="K33">
     <cfRule type="cellIs" dxfId="76" priority="163" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K34">
+  <conditionalFormatting sqref="K33">
     <cfRule type="cellIs" dxfId="75" priority="164" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K34">
+  <conditionalFormatting sqref="K33">
     <cfRule type="cellIs" dxfId="74" priority="165" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K34">
+  <conditionalFormatting sqref="K33">
     <cfRule type="cellIs" dxfId="73" priority="166" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M34">
+  <conditionalFormatting sqref="M33">
     <cfRule type="cellIs" dxfId="72" priority="161" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
@@ -7623,27 +7620,27 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L22:L23 I22:I23 G22:G23 E22:E23 C22:C23">
+  <conditionalFormatting sqref="L22 I22 G22 E22 C22">
     <cfRule type="cellIs" dxfId="55" priority="141" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C22:M23">
+  <conditionalFormatting sqref="C22:M22">
     <cfRule type="cellIs" dxfId="54" priority="142" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C22:M23">
+  <conditionalFormatting sqref="C22:M22">
     <cfRule type="cellIs" dxfId="53" priority="143" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C22:M23">
+  <conditionalFormatting sqref="C22:M22">
     <cfRule type="cellIs" dxfId="52" priority="144" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K22:K23">
+  <conditionalFormatting sqref="K22">
     <cfRule type="cellIs" dxfId="51" priority="140" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7653,7 +7650,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K30">
+  <conditionalFormatting sqref="K29">
     <cfRule type="cellIs" dxfId="49" priority="121" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -7713,132 +7710,132 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C30 E30 G30 I30 L30">
+  <conditionalFormatting sqref="C29 E29 G29 I29 L29">
     <cfRule type="cellIs" dxfId="37" priority="124" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C30:J30 L30:M30">
+  <conditionalFormatting sqref="C29:J29 L29:M29">
     <cfRule type="cellIs" dxfId="36" priority="125" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C30:J30 L30:M30">
+  <conditionalFormatting sqref="C29:J29 L29:M29">
     <cfRule type="cellIs" dxfId="35" priority="126" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C30:J30 L30:M30">
+  <conditionalFormatting sqref="C29:J29 L29:M29">
     <cfRule type="cellIs" dxfId="34" priority="127" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K30">
+  <conditionalFormatting sqref="K29">
     <cfRule type="cellIs" dxfId="33" priority="122" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K30">
+  <conditionalFormatting sqref="K29">
     <cfRule type="cellIs" dxfId="32" priority="123" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C26 E26 G26 I26 L26">
+  <conditionalFormatting sqref="C25 E25 G25 I25 L25">
     <cfRule type="cellIs" dxfId="31" priority="117" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C26:J26 L26:M26">
+  <conditionalFormatting sqref="C25:J25 L25:M25">
     <cfRule type="cellIs" dxfId="30" priority="118" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C26:J26 L26:M26">
+  <conditionalFormatting sqref="C25:J25 L25:M25">
     <cfRule type="cellIs" dxfId="29" priority="119" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C26:J26 L26:M26">
+  <conditionalFormatting sqref="C25:J25 L25:M25">
     <cfRule type="cellIs" dxfId="28" priority="120" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K26">
+  <conditionalFormatting sqref="K25">
     <cfRule type="cellIs" dxfId="27" priority="114" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K26">
+  <conditionalFormatting sqref="K25">
     <cfRule type="cellIs" dxfId="26" priority="115" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K26">
+  <conditionalFormatting sqref="K25">
     <cfRule type="cellIs" dxfId="25" priority="116" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L32">
+  <conditionalFormatting sqref="L31">
     <cfRule type="cellIs" dxfId="24" priority="101" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I31 L31 G31 E31 C31">
+  <conditionalFormatting sqref="I30 L30 G30 E30 C30">
     <cfRule type="cellIs" dxfId="23" priority="109" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C31:M31">
+  <conditionalFormatting sqref="C30:M30">
     <cfRule type="cellIs" dxfId="22" priority="110" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D31 F31 H31 J31 M31">
+  <conditionalFormatting sqref="D30 F30 H30 J30 M30">
     <cfRule type="cellIs" dxfId="21" priority="111" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C31:M31">
+  <conditionalFormatting sqref="C30:M30">
     <cfRule type="cellIs" dxfId="20" priority="112" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C31:M31">
+  <conditionalFormatting sqref="C30:M30">
     <cfRule type="cellIs" dxfId="19" priority="113" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K31">
+  <conditionalFormatting sqref="K30">
     <cfRule type="cellIs" dxfId="18" priority="107" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K31">
+  <conditionalFormatting sqref="K30">
     <cfRule type="cellIs" dxfId="17" priority="108" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N31">
+  <conditionalFormatting sqref="N30">
     <cfRule type="cellIs" dxfId="16" priority="106" operator="equal">
-      <formula>$B31</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E32">
+      <formula>$B30</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31">
     <cfRule type="cellIs" dxfId="15" priority="105" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G32">
+  <conditionalFormatting sqref="G31">
     <cfRule type="cellIs" dxfId="14" priority="104" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I32">
+  <conditionalFormatting sqref="I31">
     <cfRule type="cellIs" dxfId="13" priority="103" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K32">
+  <conditionalFormatting sqref="K31">
     <cfRule type="cellIs" dxfId="12" priority="102" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
@@ -7883,22 +7880,22 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L24">
+  <conditionalFormatting sqref="L23">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J24:M24">
+  <conditionalFormatting sqref="J23:M23">
     <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J24:M24">
+  <conditionalFormatting sqref="J23:M23">
     <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J24:M24">
+  <conditionalFormatting sqref="J23:M23">
     <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>